<commit_message>
added new 21Q3 depmap IDs
</commit_message>
<xml_diff>
--- a/inst/extdata/depmap_datasets_list.xlsx
+++ b/inst/extdata/depmap_datasets_list.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="444" uniqueCount="303">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="449" uniqueCount="308">
   <si>
     <t xml:space="preserve">Dataset</t>
   </si>
@@ -880,6 +880,9 @@
     <t xml:space="preserve">(Chronos) Batch and off-target corrected CRISPR-Cas9 gene knockout dependency data</t>
   </si>
   <si>
+    <t xml:space="preserve">EH6753</t>
+  </si>
+  <si>
     <t xml:space="preserve">17393 genes, 1032 cell lines</t>
   </si>
   <si>
@@ -892,6 +895,9 @@
     <t xml:space="preserve">copyNumber_21Q3</t>
   </si>
   <si>
+    <t xml:space="preserve">EH6754</t>
+  </si>
+  <si>
     <t xml:space="preserve">27562 genes, 1741 cell lines</t>
   </si>
   <si>
@@ -901,6 +907,9 @@
     <t xml:space="preserve">TPM_21Q3</t>
   </si>
   <si>
+    <t xml:space="preserve">EH6755</t>
+  </si>
+  <si>
     <t xml:space="preserve">19177 genes, 1377 cell lines</t>
   </si>
   <si>
@@ -910,6 +919,9 @@
     <t xml:space="preserve">mutationCalls_21Q3</t>
   </si>
   <si>
+    <t xml:space="preserve">EH6756</t>
+  </si>
+  <si>
     <t xml:space="preserve">18784 genes, 1746 cell lines</t>
   </si>
   <si>
@@ -920,6 +932,9 @@
   </si>
   <si>
     <t xml:space="preserve">Metadata for cell lines in the 21Q3 DepMap release</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EH6757</t>
   </si>
   <si>
     <t xml:space="preserve">2944 cell lines</t>
@@ -1004,13 +1019,17 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -1032,8 +1051,8 @@
   </sheetPr>
   <dimension ref="A1:H64"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A39" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A67" activeCellId="0" sqref="A67"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A41" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C65" activeCellId="0" sqref="C65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2589,8 +2608,11 @@
       <c r="B60" s="0" t="s">
         <v>285</v>
       </c>
+      <c r="C60" s="2" t="s">
+        <v>286</v>
+      </c>
       <c r="D60" s="0" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="E60" s="0" t="s">
         <v>264</v>
@@ -2599,21 +2621,24 @@
         <v>3.14</v>
       </c>
       <c r="G60" s="1" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="H60" s="0" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="B61" s="0" t="s">
         <v>22</v>
       </c>
+      <c r="C61" s="2" t="s">
+        <v>291</v>
+      </c>
       <c r="D61" s="0" t="s">
-        <v>290</v>
+        <v>292</v>
       </c>
       <c r="E61" s="0" t="s">
         <v>144</v>
@@ -2622,21 +2647,24 @@
         <v>3.14</v>
       </c>
       <c r="G61" s="1" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="H61" s="0" t="s">
-        <v>291</v>
+        <v>293</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="s">
-        <v>292</v>
+        <v>294</v>
       </c>
       <c r="B62" s="0" t="s">
         <v>34</v>
       </c>
+      <c r="C62" s="2" t="s">
+        <v>295</v>
+      </c>
       <c r="D62" s="0" t="s">
-        <v>293</v>
+        <v>296</v>
       </c>
       <c r="E62" s="0" t="s">
         <v>228</v>
@@ -2645,21 +2673,24 @@
         <v>3.14</v>
       </c>
       <c r="G62" s="1" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="H62" s="0" t="s">
-        <v>294</v>
+        <v>297</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="s">
-        <v>295</v>
+        <v>298</v>
       </c>
       <c r="B63" s="0" t="s">
         <v>182</v>
       </c>
+      <c r="C63" s="2" t="s">
+        <v>299</v>
+      </c>
       <c r="D63" s="0" t="s">
-        <v>296</v>
+        <v>300</v>
       </c>
       <c r="E63" s="0" t="s">
         <v>144</v>
@@ -2668,33 +2699,36 @@
         <v>3.14</v>
       </c>
       <c r="G63" s="1" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="H63" s="0" t="s">
-        <v>297</v>
+        <v>301</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="s">
-        <v>298</v>
+        <v>302</v>
       </c>
       <c r="B64" s="0" t="s">
-        <v>299</v>
+        <v>303</v>
+      </c>
+      <c r="C64" s="2" t="s">
+        <v>304</v>
       </c>
       <c r="D64" s="0" t="s">
-        <v>300</v>
+        <v>305</v>
       </c>
       <c r="E64" s="0" t="s">
-        <v>301</v>
+        <v>306</v>
       </c>
       <c r="F64" s="0" t="n">
         <v>3.14</v>
       </c>
       <c r="G64" s="1" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="H64" s="0" t="s">
-        <v>302</v>
+        <v>307</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
minor changes in 22Q1 EH metadata files
</commit_message>
<xml_diff>
--- a/inst/extdata/depmap_datasets_list.xlsx
+++ b/inst/extdata/depmap_datasets_list.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="417" uniqueCount="304">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="455" uniqueCount="328">
   <si>
     <t xml:space="preserve">Dataset</t>
   </si>
@@ -877,7 +877,7 @@
     <t xml:space="preserve">17386 genes, 1032 cell lines</t>
   </si>
   <si>
-    <t xml:space="preserve">Aug 21 2021</t>
+    <t xml:space="preserve">Nov 21 2021</t>
   </si>
   <si>
     <t xml:space="preserve">https://ndownloader.figshare.com/files/31315996</t>
@@ -932,6 +932,94 @@
   </si>
   <si>
     <t xml:space="preserve">https://ndownloader.figshare.com/files/31316011</t>
+  </si>
+  <si>
+    <t xml:space="preserve">crispr_22Q1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">17386 genes, 1070 cell lines</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Feb 8 2022</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://ndownloader.figshare.com/files/34008491</t>
+  </si>
+  <si>
+    <t xml:space="preserve">copyNumber_22Q1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">25368 genes, 1754 cell lines</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://ndownloader.figshare.com/files/34008428</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TPM_22Q1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">19177 genes, 1393 cell lines</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://ndownloader.figshare.com/files/34008404</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mutationCalls_22Q1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">18784 genes, 1759 cell lines</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://ndownloader.figshare.com/files/34008434</t>
+  </si>
+  <si>
+    <t xml:space="preserve">metadata_22Q1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Metadata for cell lines in the 22Q1 DepMap release</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1829 cell lines</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://ndownloader.figshare.com/files/34008503</t>
+  </si>
+  <si>
+    <t xml:space="preserve">achilles_22Q1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Project Achilles’ CRISPR screen metadata</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://ndownloader.figshare.com/files/34008386</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">gene_summary</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">_22Q1</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Gene summaries displaying probability of dependency </t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://depmap.org/portal/api/download/gene_dep_summary</t>
+  </si>
+  <si>
+    <t xml:space="preserve">drug_sensitivity_21Q2</t>
   </si>
 </sst>
 </file>
@@ -942,7 +1030,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -963,6 +1051,11 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -1037,10 +1130,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I69"/>
+  <dimension ref="A1:I77"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F2" activeCellId="0" sqref="F2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A64" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B88" activeCellId="0" sqref="B88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3058,6 +3151,196 @@
         <v>303</v>
       </c>
     </row>
+    <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A70" s="0" t="s">
+        <v>304</v>
+      </c>
+      <c r="B70" s="0" t="s">
+        <v>260</v>
+      </c>
+      <c r="D70" s="0" t="s">
+        <v>305</v>
+      </c>
+      <c r="E70" s="0" t="n">
+        <v>32</v>
+      </c>
+      <c r="F70" s="0" t="n">
+        <v>31</v>
+      </c>
+      <c r="G70" s="0" t="n">
+        <v>3.15</v>
+      </c>
+      <c r="H70" s="1" t="s">
+        <v>306</v>
+      </c>
+      <c r="I70" s="0" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A71" s="0" t="s">
+        <v>308</v>
+      </c>
+      <c r="B71" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="D71" s="0" t="s">
+        <v>309</v>
+      </c>
+      <c r="E71" s="0" t="n">
+        <v>35</v>
+      </c>
+      <c r="F71" s="0" t="n">
+        <v>38</v>
+      </c>
+      <c r="G71" s="0" t="n">
+        <v>3.15</v>
+      </c>
+      <c r="H71" s="1" t="s">
+        <v>306</v>
+      </c>
+      <c r="I71" s="0" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A72" s="0" t="s">
+        <v>311</v>
+      </c>
+      <c r="B72" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="D72" s="0" t="s">
+        <v>312</v>
+      </c>
+      <c r="E72" s="0" t="n">
+        <v>33</v>
+      </c>
+      <c r="F72" s="0" t="n">
+        <v>38</v>
+      </c>
+      <c r="G72" s="0" t="n">
+        <v>3.15</v>
+      </c>
+      <c r="H72" s="1" t="s">
+        <v>306</v>
+      </c>
+      <c r="I72" s="0" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A73" s="0" t="s">
+        <v>314</v>
+      </c>
+      <c r="B73" s="0" t="s">
+        <v>163</v>
+      </c>
+      <c r="D73" s="0" t="s">
+        <v>315</v>
+      </c>
+      <c r="E73" s="0" t="n">
+        <v>35</v>
+      </c>
+      <c r="F73" s="0" t="n">
+        <v>38</v>
+      </c>
+      <c r="G73" s="0" t="n">
+        <v>3.15</v>
+      </c>
+      <c r="H73" s="1" t="s">
+        <v>306</v>
+      </c>
+      <c r="I73" s="0" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A74" s="0" t="s">
+        <v>317</v>
+      </c>
+      <c r="B74" s="0" t="s">
+        <v>318</v>
+      </c>
+      <c r="D74" s="0" t="s">
+        <v>319</v>
+      </c>
+      <c r="E74" s="0" t="n">
+        <v>35</v>
+      </c>
+      <c r="F74" s="0" t="n">
+        <v>40</v>
+      </c>
+      <c r="G74" s="0" t="n">
+        <v>3.15</v>
+      </c>
+      <c r="H74" s="1" t="s">
+        <v>306</v>
+      </c>
+      <c r="I74" s="0" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A75" s="0" t="s">
+        <v>321</v>
+      </c>
+      <c r="B75" s="0" t="s">
+        <v>322</v>
+      </c>
+      <c r="G75" s="0" t="n">
+        <v>3.15</v>
+      </c>
+      <c r="H75" s="1" t="s">
+        <v>306</v>
+      </c>
+      <c r="I75" s="0" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A76" s="0" t="s">
+        <v>324</v>
+      </c>
+      <c r="B76" s="0" t="s">
+        <v>325</v>
+      </c>
+      <c r="G76" s="0" t="n">
+        <v>3.15</v>
+      </c>
+      <c r="H76" s="1" t="s">
+        <v>306</v>
+      </c>
+      <c r="I76" s="0" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A77" s="0" t="s">
+        <v>327</v>
+      </c>
+      <c r="B77" s="0" t="s">
+        <v>101</v>
+      </c>
+      <c r="D77" s="0" t="s">
+        <v>103</v>
+      </c>
+      <c r="E77" s="0" t="n">
+        <v>23</v>
+      </c>
+      <c r="F77" s="0" t="n">
+        <v>25</v>
+      </c>
+      <c r="G77" s="0" t="n">
+        <v>3.15</v>
+      </c>
+      <c r="H77" s="1" t="s">
+        <v>306</v>
+      </c>
+      <c r="I77" s="0" t="s">
+        <v>104</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
updated EH numbers for 22Q1 release
</commit_message>
<xml_diff>
--- a/inst/extdata/depmap_datasets_list.xlsx
+++ b/inst/extdata/depmap_datasets_list.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="455" uniqueCount="328">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="413" uniqueCount="274">
   <si>
     <t xml:space="preserve">Dataset</t>
   </si>
@@ -31,7 +31,10 @@
     <t xml:space="preserve">EH_Number</t>
   </si>
   <si>
-    <t xml:space="preserve">Dimensions</t>
+    <t xml:space="preserve">Genes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cell_Lines</t>
   </si>
   <si>
     <t xml:space="preserve">Primary_Diseases</t>
@@ -58,9 +61,6 @@
     <t xml:space="preserve">EH2260</t>
   </si>
   <si>
-    <t xml:space="preserve">17309 genes, 711 cancer cell lines</t>
-  </si>
-  <si>
     <t xml:space="preserve">Feb 19 2019</t>
   </si>
   <si>
@@ -76,9 +76,6 @@
     <t xml:space="preserve">EH2261</t>
   </si>
   <si>
-    <t xml:space="preserve">17634 genes, 558 cell lines</t>
-  </si>
-  <si>
     <t xml:space="preserve">https://ndownloader.figshare.com/files/14221385</t>
   </si>
   <si>
@@ -91,9 +88,6 @@
     <t xml:space="preserve">EH2262</t>
   </si>
   <si>
-    <t xml:space="preserve">23299 genes, 1604 cell lines</t>
-  </si>
-  <si>
     <t xml:space="preserve">https://depmap.org/portal/download/api/download/external?file_name=ccle%2Fdepmap-wes-cn-data-97cc.14%2Fpublic_19Q1_gene_cn.csv</t>
   </si>
   <si>
@@ -106,9 +100,6 @@
     <t xml:space="preserve">EH2263</t>
   </si>
   <si>
-    <t xml:space="preserve">214 genes, 899 cell lines</t>
-  </si>
-  <si>
     <t xml:space="preserve">https://depmap.org/portal/download/api/download/external?file_name=ccle%2Fdepmap-rnaseq-expression-data-ccd0.12%2FCCLE_depMap_19Q1_TPM.csv</t>
   </si>
   <si>
@@ -121,9 +112,6 @@
     <t xml:space="preserve">EH2264</t>
   </si>
   <si>
-    <t xml:space="preserve">57820 genes, 1165 cell lines</t>
-  </si>
-  <si>
     <t xml:space="preserve">https://depmap.org/portal/download/api/download/external?file_name=ccle%2FCCLE_RPPA_20180123.csv</t>
   </si>
   <si>
@@ -136,9 +124,6 @@
     <t xml:space="preserve">EH2265</t>
   </si>
   <si>
-    <t xml:space="preserve">18755 genes, 1601 cell lines</t>
-  </si>
-  <si>
     <t xml:space="preserve">https://depmap.org/portal/download/api/download/external?file_name=ccle%2Fdepmap-mutation-calls-9a1a.7%2Fdepmap_19Q1_mutation_calls.csv</t>
   </si>
   <si>
@@ -151,7 +136,7 @@
     <t xml:space="preserve">EH2266</t>
   </si>
   <si>
-    <t xml:space="preserve">1677 cell lines</t>
+    <t xml:space="preserve">NA</t>
   </si>
   <si>
     <t xml:space="preserve">https://depmap.org/portal/download/api/download/external?file_name=processed_portal_downloads%2Fdepmap-public-cell-line-metadata-183e.4%2FDepMap-2019q1-celllines_v2.csv</t>
@@ -163,9 +148,6 @@
     <t xml:space="preserve">EH2550</t>
   </si>
   <si>
-    <t xml:space="preserve">17309 genes, 712 cell lines</t>
-  </si>
-  <si>
     <t xml:space="preserve">May 7 2019</t>
   </si>
   <si>
@@ -175,9 +157,6 @@
     <t xml:space="preserve">EH2551</t>
   </si>
   <si>
-    <t xml:space="preserve">17634 genes, 563 cell lines</t>
-  </si>
-  <si>
     <t xml:space="preserve">https://ndownloader.figshare.com/files/15023465</t>
   </si>
   <si>
@@ -187,9 +166,6 @@
     <t xml:space="preserve">EH2552</t>
   </si>
   <si>
-    <t xml:space="preserve">23299 genes, 1627 cell lines</t>
-  </si>
-  <si>
     <t xml:space="preserve">https://ndownloader.figshare.com/files/15023495</t>
   </si>
   <si>
@@ -205,9 +181,6 @@
     <t xml:space="preserve">EH2554</t>
   </si>
   <si>
-    <t xml:space="preserve">19144 genes, 1165 cell lines</t>
-  </si>
-  <si>
     <t xml:space="preserve">https://ndownloader.figshare.com/files/15023483</t>
   </si>
   <si>
@@ -220,9 +193,6 @@
     <t xml:space="preserve">EH2555</t>
   </si>
   <si>
-    <t xml:space="preserve">18796 genes, 1631 cell lines</t>
-  </si>
-  <si>
     <t xml:space="preserve">https://ndownloader.figshare.com/files/15023498</t>
   </si>
   <si>
@@ -235,9 +205,6 @@
     <t xml:space="preserve">EH2556</t>
   </si>
   <si>
-    <t xml:space="preserve">1714 cell lines</t>
-  </si>
-  <si>
     <t xml:space="preserve">https://ndownloader.figshare.com/files/15023525</t>
   </si>
   <si>
@@ -256,9 +223,6 @@
     <t xml:space="preserve">EH3081</t>
   </si>
   <si>
-    <t xml:space="preserve">18333 genes, 625 cell lines</t>
-  </si>
-  <si>
     <t xml:space="preserve">https://ndownloader.figshare.com/files/16757666</t>
   </si>
   <si>
@@ -268,9 +232,6 @@
     <t xml:space="preserve">EH3082</t>
   </si>
   <si>
-    <t xml:space="preserve">27562 genes, 1657 cell lines</t>
-  </si>
-  <si>
     <t xml:space="preserve">https://ndownloader.figshare.com/files/16757699</t>
   </si>
   <si>
@@ -289,9 +250,6 @@
     <t xml:space="preserve">EH3084</t>
   </si>
   <si>
-    <t xml:space="preserve">19144 genes, 1210 cell lines</t>
-  </si>
-  <si>
     <t xml:space="preserve">https://ndownloader.figshare.com/files/16757690</t>
   </si>
   <si>
@@ -301,9 +259,6 @@
     <t xml:space="preserve">EH3085</t>
   </si>
   <si>
-    <t xml:space="preserve">18798 genes, 1656 cell lines</t>
-  </si>
-  <si>
     <t xml:space="preserve">https://ndownloader.figshare.com/files/16757702</t>
   </si>
   <si>
@@ -316,9 +271,6 @@
     <t xml:space="preserve">EH3086</t>
   </si>
   <si>
-    <t xml:space="preserve">1736 cell lines</t>
-  </si>
-  <si>
     <t xml:space="preserve">https://ndownloader.figshare.com/files/16757723</t>
   </si>
   <si>
@@ -331,9 +283,6 @@
     <t xml:space="preserve">EH3087</t>
   </si>
   <si>
-    <t xml:space="preserve">4686 compounds, 578 cell lines</t>
-  </si>
-  <si>
     <t xml:space="preserve">https://ndownloader.figshare.com/files/17008628</t>
   </si>
   <si>
@@ -343,9 +292,6 @@
     <t xml:space="preserve">EH3240</t>
   </si>
   <si>
-    <t xml:space="preserve">18333 genes, 689 cell lines</t>
-  </si>
-  <si>
     <t xml:space="preserve">Dec 20 2019</t>
   </si>
   <si>
@@ -358,9 +304,6 @@
     <t xml:space="preserve">EH3241</t>
   </si>
   <si>
-    <t xml:space="preserve">27639 genes, 1682 cell lines</t>
-  </si>
-  <si>
     <t xml:space="preserve">https://ndownloader.figshare.com/files/20234367</t>
   </si>
   <si>
@@ -370,9 +313,6 @@
     <t xml:space="preserve">EH3242</t>
   </si>
   <si>
-    <t xml:space="preserve">19144 genes, 1249 cell lines</t>
-  </si>
-  <si>
     <t xml:space="preserve">https://ndownloader.figshare.com/files/20234346</t>
   </si>
   <si>
@@ -382,9 +322,6 @@
     <t xml:space="preserve">EH3243</t>
   </si>
   <si>
-    <t xml:space="preserve">18798 genes, 1666 cell lines</t>
-  </si>
-  <si>
     <t xml:space="preserve">https://ndownloader.figshare.com/files/20274747</t>
   </si>
   <si>
@@ -397,9 +334,6 @@
     <t xml:space="preserve">EH3244</t>
   </si>
   <si>
-    <t xml:space="preserve">1756 cell lines</t>
-  </si>
-  <si>
     <t xml:space="preserve">https://ndownloader.figshare.com/files/20274744</t>
   </si>
   <si>
@@ -409,9 +343,6 @@
     <t xml:space="preserve">EH3290</t>
   </si>
   <si>
-    <t xml:space="preserve">18333 genes, 739 cell lines</t>
-  </si>
-  <si>
     <t xml:space="preserve">Feb 20 2020</t>
   </si>
   <si>
@@ -424,9 +355,6 @@
     <t xml:space="preserve">EH3291</t>
   </si>
   <si>
-    <t xml:space="preserve">27639 genes, 1713 cell lines</t>
-  </si>
-  <si>
     <t xml:space="preserve">https://ndownloader.figshare.com/files/21521964</t>
   </si>
   <si>
@@ -436,9 +364,6 @@
     <t xml:space="preserve">EH3292</t>
   </si>
   <si>
-    <t xml:space="preserve">19144 genes, 1270 cell lines</t>
-  </si>
-  <si>
     <t xml:space="preserve">https://ndownloader.figshare.com/files/21521940</t>
   </si>
   <si>
@@ -448,9 +373,6 @@
     <t xml:space="preserve">EH3293</t>
   </si>
   <si>
-    <t xml:space="preserve">18802 genes, 1697 cell lines</t>
-  </si>
-  <si>
     <t xml:space="preserve">https://ndownloader.figshare.com/files/21521967</t>
   </si>
   <si>
@@ -463,9 +385,6 @@
     <t xml:space="preserve">EH3294</t>
   </si>
   <si>
-    <t xml:space="preserve">1775 cell lines</t>
-  </si>
-  <si>
     <t xml:space="preserve">https://ndownloader.figshare.com/files/21522000</t>
   </si>
   <si>
@@ -475,9 +394,6 @@
     <t xml:space="preserve">EH3454</t>
   </si>
   <si>
-    <t xml:space="preserve">18119 genes, 769 cell lines</t>
-  </si>
-  <si>
     <t xml:space="preserve">May 20 2020</t>
   </si>
   <si>
@@ -490,9 +406,6 @@
     <t xml:space="preserve">EH3455</t>
   </si>
   <si>
-    <t xml:space="preserve">27639 genes, 1745 cell lines</t>
-  </si>
-  <si>
     <t xml:space="preserve">https://ndownloader.figshare.com/files/22629107</t>
   </si>
   <si>
@@ -502,9 +415,6 @@
     <t xml:space="preserve">EH3456</t>
   </si>
   <si>
-    <t xml:space="preserve">19144 genes, 1304 cell lines</t>
-  </si>
-  <si>
     <t xml:space="preserve">https://ndownloader.figshare.com/files/22629092</t>
   </si>
   <si>
@@ -517,9 +427,6 @@
     <t xml:space="preserve">EH3457</t>
   </si>
   <si>
-    <t xml:space="preserve">18802 genes, 1741 cell lines</t>
-  </si>
-  <si>
     <t xml:space="preserve">https://ndownloader.figshare.com/files/22629110</t>
   </si>
   <si>
@@ -532,9 +439,6 @@
     <t xml:space="preserve">EH3458</t>
   </si>
   <si>
-    <t xml:space="preserve">1804 cell lines</t>
-  </si>
-  <si>
     <t xml:space="preserve">https://ndownloader.figshare.com/files/22629137</t>
   </si>
   <si>
@@ -547,9 +451,6 @@
     <t xml:space="preserve">EH3459</t>
   </si>
   <si>
-    <t xml:space="preserve">12399 proteins, 375 cell lines</t>
-  </si>
-  <si>
     <t xml:space="preserve">https://gygi.med.harvard.edu/sites/gygi.med.harvard.edu/files/documents/protein_quant_current_normalized.csv.gz</t>
   </si>
   <si>
@@ -610,9 +511,6 @@
     <t xml:space="preserve">EH3960</t>
   </si>
   <si>
-    <t xml:space="preserve">18119 genes, 808 cell lines</t>
-  </si>
-  <si>
     <t xml:space="preserve">Nov 20 2020</t>
   </si>
   <si>
@@ -625,9 +523,6 @@
     <t xml:space="preserve">EH3961</t>
   </si>
   <si>
-    <t xml:space="preserve">27562 genes, 1753 cell lines</t>
-  </si>
-  <si>
     <t xml:space="preserve">https://ndownloader.figshare.com/files/25494416</t>
   </si>
   <si>
@@ -637,9 +532,6 @@
     <t xml:space="preserve">EH3962</t>
   </si>
   <si>
-    <t xml:space="preserve">19182 genes, 1376 cell lines</t>
-  </si>
-  <si>
     <t xml:space="preserve">https://ndownloader.figshare.com/files/25494389</t>
   </si>
   <si>
@@ -649,9 +541,6 @@
     <t xml:space="preserve">EH3963</t>
   </si>
   <si>
-    <t xml:space="preserve">18789 genes, 1749 cell lines</t>
-  </si>
-  <si>
     <t xml:space="preserve">https://ndownloader.figshare.com/files/25494419</t>
   </si>
   <si>
@@ -664,9 +553,6 @@
     <t xml:space="preserve">EH3964</t>
   </si>
   <si>
-    <t xml:space="preserve">1812 cell lines</t>
-  </si>
-  <si>
     <t xml:space="preserve">https://ndownloader.figshare.com/files/25494443</t>
   </si>
   <si>
@@ -688,9 +574,6 @@
     <t xml:space="preserve">EH5359</t>
   </si>
   <si>
-    <t xml:space="preserve">27562 genes, 1740 cell lines</t>
-  </si>
-  <si>
     <t xml:space="preserve">https://ndownloader.figshare.com/files/26261524</t>
   </si>
   <si>
@@ -700,9 +583,6 @@
     <t xml:space="preserve">EH5360</t>
   </si>
   <si>
-    <t xml:space="preserve">19177 genes, 1376 cell lines</t>
-  </si>
-  <si>
     <t xml:space="preserve">https://ndownloader.figshare.com/files/26261476</t>
   </si>
   <si>
@@ -712,9 +592,6 @@
     <t xml:space="preserve">EH5361</t>
   </si>
   <si>
-    <t xml:space="preserve">18788 genes, 1747 cell lines</t>
-  </si>
-  <si>
     <t xml:space="preserve">https://ndownloader.figshare.com/files/26261527</t>
   </si>
   <si>
@@ -727,9 +604,6 @@
     <t xml:space="preserve">EH5362</t>
   </si>
   <si>
-    <t xml:space="preserve">1811 cell lines</t>
-  </si>
-  <si>
     <t xml:space="preserve">https://ndownloader.figshare.com/files/26261569</t>
   </si>
   <si>
@@ -739,9 +613,6 @@
     <t xml:space="preserve">EH6118</t>
   </si>
   <si>
-    <t xml:space="preserve">17645 genes, 990 cell lines</t>
-  </si>
-  <si>
     <t xml:space="preserve">May 07 2021</t>
   </si>
   <si>
@@ -754,9 +625,6 @@
     <t xml:space="preserve">EH6119</t>
   </si>
   <si>
-    <t xml:space="preserve">27562 genes, 1742 cell lines</t>
-  </si>
-  <si>
     <t xml:space="preserve">https://ndownloader.figshare.com/files/27902124</t>
   </si>
   <si>
@@ -766,9 +634,6 @@
     <t xml:space="preserve">EH6120</t>
   </si>
   <si>
-    <t xml:space="preserve">19177 genes, 1379 cell lines</t>
-  </si>
-  <si>
     <t xml:space="preserve">https://ndownloader.figshare.com/files/27902091</t>
   </si>
   <si>
@@ -778,9 +643,6 @@
     <t xml:space="preserve">EH6121</t>
   </si>
   <si>
-    <t xml:space="preserve">18787 genes, 1750 cell lines</t>
-  </si>
-  <si>
     <t xml:space="preserve">https://ndownloader.figshare.com/files/27902118</t>
   </si>
   <si>
@@ -793,9 +655,6 @@
     <t xml:space="preserve">EH6122</t>
   </si>
   <si>
-    <t xml:space="preserve">1814 cell lines</t>
-  </si>
-  <si>
     <t xml:space="preserve">https://ndownloader.figshare.com/files/27902376</t>
   </si>
   <si>
@@ -808,9 +667,6 @@
     <t xml:space="preserve">EH6753</t>
   </si>
   <si>
-    <t xml:space="preserve">17393 genes, 1032 cell lines</t>
-  </si>
-  <si>
     <t xml:space="preserve">Aug 20 2021</t>
   </si>
   <si>
@@ -823,9 +679,6 @@
     <t xml:space="preserve">EH6754</t>
   </si>
   <si>
-    <t xml:space="preserve">27562 genes, 1741 cell lines</t>
-  </si>
-  <si>
     <t xml:space="preserve">https://ndownloader.figshare.com/files/29125230</t>
   </si>
   <si>
@@ -835,9 +688,6 @@
     <t xml:space="preserve">EH6755</t>
   </si>
   <si>
-    <t xml:space="preserve">19177 genes, 1377 cell lines</t>
-  </si>
-  <si>
     <t xml:space="preserve">https://ndownloader.figshare.com/files/29124747</t>
   </si>
   <si>
@@ -847,9 +697,6 @@
     <t xml:space="preserve">EH6756</t>
   </si>
   <si>
-    <t xml:space="preserve">18784 genes, 1746 cell lines</t>
-  </si>
-  <si>
     <t xml:space="preserve">https://ndownloader.figshare.com/files/29125233</t>
   </si>
   <si>
@@ -862,9 +709,6 @@
     <t xml:space="preserve">EH6757</t>
   </si>
   <si>
-    <t xml:space="preserve">2944 cell lines</t>
-  </si>
-  <si>
     <t xml:space="preserve">https://ndownloader.figshare.com/files/29162481</t>
   </si>
   <si>
@@ -874,9 +718,6 @@
     <t xml:space="preserve">EH7290</t>
   </si>
   <si>
-    <t xml:space="preserve">17386 genes, 1032 cell lines</t>
-  </si>
-  <si>
     <t xml:space="preserve">Nov 21 2021</t>
   </si>
   <si>
@@ -889,9 +730,6 @@
     <t xml:space="preserve">EH7291</t>
   </si>
   <si>
-    <t xml:space="preserve">25368 genes, 1750 cell lines</t>
-  </si>
-  <si>
     <t xml:space="preserve">https://ndownloader.figshare.com/files/31315924</t>
   </si>
   <si>
@@ -901,9 +739,6 @@
     <t xml:space="preserve">EH7292</t>
   </si>
   <si>
-    <t xml:space="preserve">19177 genes, 1389 cell lines</t>
-  </si>
-  <si>
     <t xml:space="preserve">https://ndownloader.figshare.com/files/31315882</t>
   </si>
   <si>
@@ -913,9 +748,6 @@
     <t xml:space="preserve">EH7293</t>
   </si>
   <si>
-    <t xml:space="preserve">18784 genes, 1755 cell lines</t>
-  </si>
-  <si>
     <t xml:space="preserve">https://ndownloader.figshare.com/files/31315930</t>
   </si>
   <si>
@@ -928,16 +760,13 @@
     <t xml:space="preserve">EH7294</t>
   </si>
   <si>
-    <t xml:space="preserve">1825 cell lines</t>
-  </si>
-  <si>
     <t xml:space="preserve">https://ndownloader.figshare.com/files/31316011</t>
   </si>
   <si>
     <t xml:space="preserve">crispr_22Q1</t>
   </si>
   <si>
-    <t xml:space="preserve">17386 genes, 1070 cell lines</t>
+    <t xml:space="preserve">EH7523</t>
   </si>
   <si>
     <t xml:space="preserve">Feb 8 2022</t>
@@ -949,7 +778,7 @@
     <t xml:space="preserve">copyNumber_22Q1</t>
   </si>
   <si>
-    <t xml:space="preserve">25368 genes, 1754 cell lines</t>
+    <t xml:space="preserve">EH7524</t>
   </si>
   <si>
     <t xml:space="preserve">https://ndownloader.figshare.com/files/34008428</t>
@@ -958,7 +787,7 @@
     <t xml:space="preserve">TPM_22Q1</t>
   </si>
   <si>
-    <t xml:space="preserve">19177 genes, 1393 cell lines</t>
+    <t xml:space="preserve">EH7525</t>
   </si>
   <si>
     <t xml:space="preserve">https://ndownloader.figshare.com/files/34008404</t>
@@ -967,7 +796,7 @@
     <t xml:space="preserve">mutationCalls_22Q1</t>
   </si>
   <si>
-    <t xml:space="preserve">18784 genes, 1759 cell lines</t>
+    <t xml:space="preserve">EH7526</t>
   </si>
   <si>
     <t xml:space="preserve">https://ndownloader.figshare.com/files/34008434</t>
@@ -979,7 +808,7 @@
     <t xml:space="preserve">Metadata for cell lines in the 22Q1 DepMap release</t>
   </si>
   <si>
-    <t xml:space="preserve">1829 cell lines</t>
+    <t xml:space="preserve">EH7527</t>
   </si>
   <si>
     <t xml:space="preserve">https://ndownloader.figshare.com/files/34008503</t>
@@ -991,35 +820,28 @@
     <t xml:space="preserve">Project Achilles’ CRISPR screen metadata</t>
   </si>
   <si>
+    <t xml:space="preserve">EH7528</t>
+  </si>
+  <si>
     <t xml:space="preserve">https://ndownloader.figshare.com/files/34008386</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">gene_summary</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">_22Q1</t>
-    </r>
+    <t xml:space="preserve">gene_summary_22Q1</t>
   </si>
   <si>
     <t xml:space="preserve">Gene summaries displaying probability of dependency </t>
   </si>
   <si>
+    <t xml:space="preserve">EH7529</t>
+  </si>
+  <si>
     <t xml:space="preserve">https://depmap.org/portal/api/download/gene_dep_summary</t>
   </si>
   <si>
     <t xml:space="preserve">drug_sensitivity_21Q2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EH7530</t>
   </si>
 </sst>
 </file>
@@ -1054,8 +876,9 @@
     </font>
     <font>
       <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
+      <name val="1682Arial"/>
+      <family val="0"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -1100,12 +923,16 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1130,10 +957,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I77"/>
+  <dimension ref="A1:J77"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A64" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B88" activeCellId="0" sqref="B88"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A52" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C75" activeCellId="0" sqref="C75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1141,13 +968,14 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.49"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="77.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="11.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="29.31"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="15.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="8.06"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="11.16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="13.24"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="147.18"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="10" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="11.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="10.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="15.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="8.06"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="11.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="13.24"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="147.18"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="11" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1178,33 +1006,39 @@
       <c r="I1" s="0" t="s">
         <v>8</v>
       </c>
+      <c r="J1" s="0" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="D2" s="0" t="s">
         <v>12</v>
       </c>
+      <c r="D2" s="0" t="n">
+        <v>17309</v>
+      </c>
       <c r="E2" s="0" t="n">
+        <v>711</v>
+      </c>
+      <c r="F2" s="0" t="n">
         <v>30</v>
       </c>
-      <c r="F2" s="0" t="n">
+      <c r="G2" s="0" t="n">
         <v>31</v>
       </c>
-      <c r="G2" s="0" t="n">
+      <c r="H2" s="0" t="n">
         <v>3.1</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="I2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="I2" s="0" t="s">
+      <c r="J2" s="0" t="s">
         <v>14</v>
       </c>
     </row>
@@ -1218,2127 +1052,2394 @@
       <c r="C3" s="0" t="s">
         <v>17</v>
       </c>
-      <c r="D3" s="0" t="s">
+      <c r="D3" s="0" t="n">
+        <v>17634</v>
+      </c>
+      <c r="E3" s="0" t="n">
+        <v>558</v>
+      </c>
+      <c r="F3" s="0" t="n">
+        <v>26</v>
+      </c>
+      <c r="G3" s="0" t="n">
+        <v>28</v>
+      </c>
+      <c r="H3" s="0" t="n">
+        <v>3.1</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J3" s="0" t="s">
         <v>18</v>
-      </c>
-      <c r="E3" s="0" t="n">
-        <v>26</v>
-      </c>
-      <c r="F3" s="0" t="n">
-        <v>28</v>
-      </c>
-      <c r="G3" s="0" t="n">
-        <v>3.1</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="I3" s="0" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="C4" s="0" t="s">
         <v>21</v>
       </c>
-      <c r="C4" s="0" t="s">
+      <c r="D4" s="0" t="n">
+        <v>23299</v>
+      </c>
+      <c r="E4" s="0" t="n">
+        <v>1604</v>
+      </c>
+      <c r="F4" s="0" t="n">
+        <v>38</v>
+      </c>
+      <c r="G4" s="0" t="n">
+        <v>33</v>
+      </c>
+      <c r="H4" s="0" t="n">
+        <v>3.1</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J4" s="0" t="s">
         <v>22</v>
-      </c>
-      <c r="D4" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="E4" s="0" t="n">
-        <v>38</v>
-      </c>
-      <c r="F4" s="0" t="n">
-        <v>33</v>
-      </c>
-      <c r="G4" s="0" t="n">
-        <v>3.1</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="I4" s="0" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="C5" s="0" t="s">
         <v>25</v>
       </c>
-      <c r="B5" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="C5" s="0" t="s">
-        <v>27</v>
-      </c>
-      <c r="D5" s="0" t="s">
-        <v>28</v>
+      <c r="D5" s="0" t="n">
+        <v>214</v>
       </c>
       <c r="E5" s="0" t="n">
-        <v>28</v>
+        <v>899</v>
       </c>
       <c r="F5" s="0" t="n">
         <v>28</v>
       </c>
       <c r="G5" s="0" t="n">
+        <v>28</v>
+      </c>
+      <c r="H5" s="0" t="n">
         <v>3.1</v>
       </c>
-      <c r="H5" s="1" t="s">
+      <c r="I5" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="I5" s="0" t="s">
-        <v>29</v>
+      <c r="J5" s="0" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="D6" s="0" t="n">
+        <v>57820</v>
+      </c>
+      <c r="E6" s="0" t="n">
+        <v>1165</v>
+      </c>
+      <c r="F6" s="0" t="n">
+        <v>33</v>
+      </c>
+      <c r="G6" s="0" t="n">
+        <v>32</v>
+      </c>
+      <c r="H6" s="0" t="n">
+        <v>3.1</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J6" s="0" t="s">
         <v>30</v>
-      </c>
-      <c r="B6" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="C6" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="D6" s="0" t="s">
-        <v>33</v>
-      </c>
-      <c r="E6" s="0" t="n">
-        <v>33</v>
-      </c>
-      <c r="F6" s="0" t="n">
-        <v>32</v>
-      </c>
-      <c r="G6" s="0" t="n">
-        <v>3.1</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="I6" s="0" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>37</v>
-      </c>
-      <c r="D7" s="0" t="s">
-        <v>38</v>
+        <v>33</v>
+      </c>
+      <c r="D7" s="0" t="n">
+        <v>18755</v>
       </c>
       <c r="E7" s="0" t="n">
-        <v>37</v>
+        <v>1601</v>
       </c>
       <c r="F7" s="0" t="n">
         <v>37</v>
       </c>
       <c r="G7" s="0" t="n">
+        <v>37</v>
+      </c>
+      <c r="H7" s="0" t="n">
         <v>3.1</v>
       </c>
-      <c r="H7" s="1" t="s">
+      <c r="I7" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="I7" s="0" t="s">
-        <v>39</v>
+      <c r="J7" s="0" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="E8" s="0" t="n">
-        <v>38</v>
+        <v>1677</v>
       </c>
       <c r="F8" s="0" t="n">
+        <v>38</v>
+      </c>
+      <c r="G8" s="0" t="n">
         <v>33</v>
       </c>
-      <c r="G8" s="0" t="n">
+      <c r="H8" s="0" t="n">
         <v>3.1</v>
       </c>
-      <c r="H8" s="1" t="s">
+      <c r="I8" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="I8" s="0" t="s">
-        <v>44</v>
+      <c r="J8" s="0" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>46</v>
-      </c>
-      <c r="D9" s="0" t="s">
-        <v>47</v>
+        <v>41</v>
+      </c>
+      <c r="D9" s="0" t="n">
+        <v>17309</v>
       </c>
       <c r="E9" s="0" t="n">
+        <v>712</v>
+      </c>
+      <c r="F9" s="0" t="n">
         <v>30</v>
       </c>
-      <c r="F9" s="0" t="n">
+      <c r="G9" s="0" t="n">
         <v>31</v>
       </c>
-      <c r="G9" s="0" t="n">
+      <c r="H9" s="0" t="n">
         <v>3.1</v>
       </c>
-      <c r="H9" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="I9" s="0" t="s">
+      <c r="I9" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="J9" s="0" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="B10" s="0" t="s">
         <v>16</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>50</v>
-      </c>
-      <c r="D10" s="0" t="s">
-        <v>51</v>
+        <v>44</v>
+      </c>
+      <c r="D10" s="0" t="n">
+        <v>17634</v>
       </c>
       <c r="E10" s="0" t="n">
+        <v>563</v>
+      </c>
+      <c r="F10" s="0" t="n">
         <v>27</v>
       </c>
-      <c r="F10" s="0" t="n">
+      <c r="G10" s="0" t="n">
         <v>29</v>
       </c>
-      <c r="G10" s="0" t="n">
+      <c r="H10" s="0" t="n">
         <v>3.1</v>
       </c>
-      <c r="H10" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="I10" s="0" t="s">
-        <v>52</v>
+      <c r="I10" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="J10" s="0" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>54</v>
-      </c>
-      <c r="D11" s="0" t="s">
-        <v>55</v>
+        <v>47</v>
+      </c>
+      <c r="D11" s="0" t="n">
+        <v>23299</v>
       </c>
       <c r="E11" s="0" t="n">
-        <v>38</v>
+        <v>1627</v>
       </c>
       <c r="F11" s="0" t="n">
+        <v>38</v>
+      </c>
+      <c r="G11" s="0" t="n">
         <v>34</v>
       </c>
-      <c r="G11" s="0" t="n">
+      <c r="H11" s="0" t="n">
         <v>3.1</v>
       </c>
-      <c r="H11" s="1" t="s">
+      <c r="I11" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="J11" s="0" t="s">
         <v>48</v>
-      </c>
-      <c r="I11" s="0" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>58</v>
-      </c>
-      <c r="D12" s="0" t="s">
-        <v>28</v>
+        <v>50</v>
+      </c>
+      <c r="D12" s="0" t="n">
+        <v>214</v>
       </c>
       <c r="E12" s="0" t="n">
-        <v>28</v>
+        <v>899</v>
       </c>
       <c r="F12" s="0" t="n">
         <v>28</v>
       </c>
       <c r="G12" s="0" t="n">
+        <v>28</v>
+      </c>
+      <c r="H12" s="0" t="n">
         <v>3.1</v>
       </c>
-      <c r="H12" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="I12" s="0" t="s">
-        <v>34</v>
+      <c r="I12" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="J12" s="0" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>60</v>
-      </c>
-      <c r="D13" s="0" t="s">
-        <v>61</v>
+        <v>52</v>
+      </c>
+      <c r="D13" s="0" t="n">
+        <v>19144</v>
       </c>
       <c r="E13" s="0" t="n">
+        <v>1165</v>
+      </c>
+      <c r="F13" s="0" t="n">
         <v>34</v>
       </c>
-      <c r="F13" s="0" t="n">
+      <c r="G13" s="0" t="n">
         <v>33</v>
       </c>
-      <c r="G13" s="0" t="n">
+      <c r="H13" s="0" t="n">
         <v>3.1</v>
       </c>
-      <c r="H13" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="I13" s="0" t="s">
-        <v>62</v>
+      <c r="I13" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="J13" s="0" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>65</v>
-      </c>
-      <c r="D14" s="0" t="s">
-        <v>66</v>
+        <v>56</v>
+      </c>
+      <c r="D14" s="0" t="n">
+        <v>18796</v>
       </c>
       <c r="E14" s="0" t="n">
+        <v>1631</v>
+      </c>
+      <c r="F14" s="0" t="n">
         <v>37</v>
       </c>
-      <c r="F14" s="0" t="n">
+      <c r="G14" s="0" t="n">
         <v>34</v>
       </c>
-      <c r="G14" s="0" t="n">
+      <c r="H14" s="0" t="n">
         <v>3.1</v>
       </c>
-      <c r="H14" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="I14" s="0" t="s">
-        <v>67</v>
+      <c r="I14" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="J14" s="0" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>68</v>
+        <v>58</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>71</v>
+        <v>38</v>
       </c>
       <c r="E15" s="0" t="n">
+        <v>1714</v>
+      </c>
+      <c r="F15" s="0" t="n">
         <v>39</v>
       </c>
-      <c r="F15" s="0" t="n">
+      <c r="G15" s="0" t="n">
         <v>34</v>
       </c>
-      <c r="G15" s="0" t="n">
+      <c r="H15" s="0" t="n">
         <v>3.1</v>
       </c>
-      <c r="H15" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="I15" s="0" t="s">
-        <v>72</v>
+      <c r="I15" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="J15" s="0" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>73</v>
+        <v>62</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>74</v>
-      </c>
-      <c r="D16" s="0" t="s">
-        <v>47</v>
+        <v>63</v>
+      </c>
+      <c r="D16" s="0" t="n">
+        <v>17309</v>
       </c>
       <c r="E16" s="0" t="n">
-        <v>31</v>
+        <v>712</v>
       </c>
       <c r="F16" s="0" t="n">
         <v>31</v>
       </c>
       <c r="G16" s="0" t="n">
+        <v>31</v>
+      </c>
+      <c r="H16" s="0" t="n">
         <v>3.1</v>
       </c>
-      <c r="H16" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="I16" s="0" t="s">
+      <c r="I16" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="J16" s="0" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>76</v>
+        <v>65</v>
       </c>
       <c r="B17" s="0" t="s">
         <v>16</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>77</v>
-      </c>
-      <c r="D17" s="0" t="s">
-        <v>78</v>
+        <v>66</v>
+      </c>
+      <c r="D17" s="0" t="n">
+        <v>18333</v>
       </c>
       <c r="E17" s="0" t="n">
+        <v>625</v>
+      </c>
+      <c r="F17" s="0" t="n">
         <v>28</v>
       </c>
-      <c r="F17" s="0" t="n">
+      <c r="G17" s="0" t="n">
         <v>29</v>
       </c>
-      <c r="G17" s="0" t="n">
+      <c r="H17" s="0" t="n">
         <v>3.1</v>
       </c>
-      <c r="H17" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="I17" s="0" t="s">
-        <v>79</v>
+      <c r="I17" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="J17" s="0" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>80</v>
+        <v>68</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>81</v>
-      </c>
-      <c r="D18" s="0" t="s">
-        <v>82</v>
+        <v>69</v>
+      </c>
+      <c r="D18" s="0" t="n">
+        <v>27562</v>
       </c>
       <c r="E18" s="0" t="n">
+        <v>1657</v>
+      </c>
+      <c r="F18" s="0" t="n">
         <v>36</v>
       </c>
-      <c r="F18" s="0" t="n">
+      <c r="G18" s="0" t="n">
         <v>34</v>
       </c>
-      <c r="G18" s="0" t="n">
+      <c r="H18" s="0" t="n">
         <v>3.1</v>
       </c>
-      <c r="H18" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="I18" s="0" t="s">
-        <v>83</v>
+      <c r="I18" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="J18" s="0" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>84</v>
+        <v>71</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>85</v>
-      </c>
-      <c r="D19" s="0" t="s">
-        <v>28</v>
+        <v>72</v>
+      </c>
+      <c r="D19" s="0" t="n">
+        <v>214</v>
       </c>
       <c r="E19" s="0" t="n">
-        <v>28</v>
+        <v>899</v>
       </c>
       <c r="F19" s="0" t="n">
         <v>28</v>
       </c>
       <c r="G19" s="0" t="n">
+        <v>28</v>
+      </c>
+      <c r="H19" s="0" t="n">
         <v>3.1</v>
       </c>
-      <c r="H19" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="I19" s="0" t="s">
-        <v>86</v>
+      <c r="I19" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="J19" s="0" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>87</v>
+        <v>74</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>88</v>
-      </c>
-      <c r="D20" s="0" t="s">
-        <v>89</v>
+        <v>75</v>
+      </c>
+      <c r="D20" s="0" t="n">
+        <v>19144</v>
       </c>
       <c r="E20" s="0" t="n">
+        <v>1210</v>
+      </c>
+      <c r="F20" s="0" t="n">
         <v>32</v>
       </c>
-      <c r="F20" s="0" t="n">
+      <c r="G20" s="0" t="n">
         <v>33</v>
       </c>
-      <c r="G20" s="0" t="n">
+      <c r="H20" s="0" t="n">
         <v>3.1</v>
       </c>
-      <c r="H20" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="I20" s="0" t="s">
-        <v>90</v>
+      <c r="I20" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="J20" s="0" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>91</v>
+        <v>77</v>
       </c>
       <c r="B21" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="C21" s="0" t="s">
+        <v>78</v>
+      </c>
+      <c r="D21" s="0" t="n">
+        <v>18798</v>
+      </c>
+      <c r="E21" s="0" t="n">
+        <v>1656</v>
+      </c>
+      <c r="F21" s="0" t="n">
         <v>36</v>
       </c>
-      <c r="C21" s="0" t="s">
-        <v>92</v>
-      </c>
-      <c r="D21" s="0" t="s">
-        <v>93</v>
-      </c>
-      <c r="E21" s="0" t="n">
-        <v>36</v>
-      </c>
-      <c r="F21" s="0" t="n">
+      <c r="G21" s="0" t="n">
         <v>34</v>
       </c>
-      <c r="G21" s="0" t="n">
+      <c r="H21" s="0" t="n">
         <v>3.1</v>
       </c>
-      <c r="H21" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="I21" s="0" t="s">
-        <v>94</v>
+      <c r="I21" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="J21" s="0" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>95</v>
+        <v>80</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>96</v>
+        <v>81</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>97</v>
+        <v>82</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>98</v>
+        <v>38</v>
       </c>
       <c r="E22" s="0" t="n">
+        <v>1736</v>
+      </c>
+      <c r="F22" s="0" t="n">
         <v>37</v>
       </c>
-      <c r="F22" s="0" t="n">
+      <c r="G22" s="0" t="n">
         <v>34</v>
       </c>
-      <c r="G22" s="0" t="n">
+      <c r="H22" s="0" t="n">
         <v>3.1</v>
       </c>
-      <c r="H22" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="I22" s="0" t="s">
-        <v>99</v>
+      <c r="I22" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="J22" s="0" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>100</v>
+        <v>84</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>101</v>
+        <v>85</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>102</v>
+        <v>86</v>
       </c>
       <c r="D23" s="0" t="s">
-        <v>103</v>
+        <v>38</v>
       </c>
       <c r="E23" s="0" t="n">
+        <v>578</v>
+      </c>
+      <c r="F23" s="0" t="n">
         <v>23</v>
       </c>
-      <c r="F23" s="0" t="n">
+      <c r="G23" s="0" t="n">
         <v>25</v>
       </c>
-      <c r="G23" s="0" t="n">
+      <c r="H23" s="0" t="n">
         <v>3.1</v>
       </c>
-      <c r="H23" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="I23" s="0" t="s">
-        <v>104</v>
+      <c r="I23" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="J23" s="0" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>105</v>
+        <v>88</v>
       </c>
       <c r="B24" s="0" t="s">
         <v>16</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>106</v>
-      </c>
-      <c r="D24" s="0" t="s">
-        <v>107</v>
+        <v>89</v>
+      </c>
+      <c r="D24" s="0" t="n">
+        <v>18333</v>
       </c>
       <c r="E24" s="0" t="n">
+        <v>689</v>
+      </c>
+      <c r="F24" s="0" t="n">
         <v>29</v>
       </c>
-      <c r="F24" s="0" t="n">
+      <c r="G24" s="0" t="n">
         <v>26</v>
       </c>
-      <c r="G24" s="0" t="n">
+      <c r="H24" s="0" t="n">
         <v>3.11</v>
       </c>
-      <c r="H24" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="I24" s="0" t="s">
-        <v>109</v>
+      <c r="I24" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="J24" s="0" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>110</v>
+        <v>92</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>111</v>
-      </c>
-      <c r="D25" s="0" t="s">
-        <v>112</v>
-      </c>
-      <c r="E25" s="0" t="n">
+        <v>93</v>
+      </c>
+      <c r="D25" s="0" t="n">
+        <v>27639</v>
+      </c>
+      <c r="E25" s="2" t="n">
+        <v>1682</v>
+      </c>
+      <c r="F25" s="0" t="n">
         <v>35</v>
       </c>
-      <c r="F25" s="0" t="n">
+      <c r="G25" s="0" t="n">
         <v>36</v>
       </c>
-      <c r="G25" s="0" t="n">
+      <c r="H25" s="0" t="n">
         <v>3.11</v>
       </c>
-      <c r="H25" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="I25" s="0" t="s">
-        <v>113</v>
+      <c r="I25" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="J25" s="0" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>114</v>
+        <v>95</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C26" s="0" t="s">
-        <v>115</v>
-      </c>
-      <c r="D26" s="0" t="s">
-        <v>116</v>
+        <v>96</v>
+      </c>
+      <c r="D26" s="0" t="n">
+        <v>19144</v>
       </c>
       <c r="E26" s="0" t="n">
+        <v>1249</v>
+      </c>
+      <c r="F26" s="0" t="n">
         <v>32</v>
       </c>
-      <c r="F26" s="0" t="n">
+      <c r="G26" s="0" t="n">
         <v>34</v>
       </c>
-      <c r="G26" s="0" t="n">
+      <c r="H26" s="0" t="n">
         <v>3.11</v>
       </c>
-      <c r="H26" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="I26" s="0" t="s">
-        <v>117</v>
+      <c r="I26" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="J26" s="0" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>118</v>
+        <v>98</v>
       </c>
       <c r="B27" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="C27" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="D27" s="0" t="n">
+        <v>18798</v>
+      </c>
+      <c r="E27" s="0" t="n">
+        <v>1666</v>
+      </c>
+      <c r="F27" s="0" t="n">
+        <v>35</v>
+      </c>
+      <c r="G27" s="0" t="n">
         <v>36</v>
       </c>
-      <c r="C27" s="0" t="s">
-        <v>119</v>
-      </c>
-      <c r="D27" s="0" t="s">
-        <v>120</v>
-      </c>
-      <c r="E27" s="0" t="n">
-        <v>35</v>
-      </c>
-      <c r="F27" s="0" t="n">
-        <v>36</v>
-      </c>
-      <c r="G27" s="0" t="n">
+      <c r="H27" s="0" t="n">
         <v>3.11</v>
       </c>
-      <c r="H27" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="I27" s="0" t="s">
-        <v>121</v>
+      <c r="I27" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="J27" s="0" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>122</v>
+        <v>101</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>123</v>
+        <v>102</v>
       </c>
       <c r="C28" s="0" t="s">
-        <v>124</v>
+        <v>103</v>
       </c>
       <c r="D28" s="0" t="s">
-        <v>125</v>
+        <v>38</v>
       </c>
       <c r="E28" s="0" t="n">
+        <v>1756</v>
+      </c>
+      <c r="F28" s="0" t="n">
         <v>35</v>
       </c>
-      <c r="F28" s="0" t="n">
+      <c r="G28" s="0" t="n">
         <v>37</v>
       </c>
-      <c r="G28" s="0" t="n">
+      <c r="H28" s="0" t="n">
         <v>3.11</v>
       </c>
-      <c r="H28" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="I28" s="0" t="s">
-        <v>126</v>
+      <c r="I28" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="J28" s="0" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>127</v>
+        <v>105</v>
       </c>
       <c r="B29" s="0" t="s">
         <v>16</v>
       </c>
       <c r="C29" s="0" t="s">
-        <v>128</v>
-      </c>
-      <c r="D29" s="0" t="s">
-        <v>129</v>
+        <v>106</v>
+      </c>
+      <c r="D29" s="0" t="n">
+        <v>18333</v>
       </c>
       <c r="E29" s="0" t="n">
+        <v>739</v>
+      </c>
+      <c r="F29" s="0" t="n">
         <v>29</v>
       </c>
-      <c r="F29" s="0" t="n">
+      <c r="G29" s="0" t="n">
         <v>26</v>
       </c>
-      <c r="G29" s="0" t="n">
+      <c r="H29" s="0" t="n">
         <v>3.12</v>
       </c>
-      <c r="H29" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="I29" s="0" t="s">
-        <v>131</v>
+      <c r="I29" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="J29" s="0" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>132</v>
+        <v>109</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C30" s="0" t="s">
-        <v>133</v>
-      </c>
-      <c r="D30" s="0" t="s">
-        <v>134</v>
+        <v>110</v>
+      </c>
+      <c r="D30" s="0" t="n">
+        <v>27639</v>
       </c>
       <c r="E30" s="0" t="n">
+        <v>1713</v>
+      </c>
+      <c r="F30" s="0" t="n">
         <v>35</v>
       </c>
-      <c r="F30" s="0" t="n">
+      <c r="G30" s="0" t="n">
         <v>36</v>
       </c>
-      <c r="G30" s="0" t="n">
+      <c r="H30" s="0" t="n">
         <v>3.12</v>
       </c>
-      <c r="H30" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="I30" s="0" t="s">
-        <v>135</v>
+      <c r="I30" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="J30" s="0" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>136</v>
+        <v>112</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C31" s="0" t="s">
-        <v>137</v>
-      </c>
-      <c r="D31" s="0" t="s">
-        <v>138</v>
+        <v>113</v>
+      </c>
+      <c r="D31" s="0" t="n">
+        <v>19144</v>
       </c>
       <c r="E31" s="0" t="n">
+        <v>1270</v>
+      </c>
+      <c r="F31" s="0" t="n">
         <v>32</v>
       </c>
-      <c r="F31" s="0" t="n">
+      <c r="G31" s="0" t="n">
         <v>34</v>
       </c>
-      <c r="G31" s="0" t="n">
+      <c r="H31" s="0" t="n">
         <v>3.12</v>
       </c>
-      <c r="H31" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="I31" s="0" t="s">
-        <v>139</v>
+      <c r="I31" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="J31" s="0" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>140</v>
+        <v>115</v>
       </c>
       <c r="B32" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="C32" s="0" t="s">
+        <v>116</v>
+      </c>
+      <c r="D32" s="0" t="n">
+        <v>18802</v>
+      </c>
+      <c r="E32" s="0" t="n">
+        <v>1697</v>
+      </c>
+      <c r="F32" s="0" t="n">
+        <v>35</v>
+      </c>
+      <c r="G32" s="0" t="n">
         <v>36</v>
       </c>
-      <c r="C32" s="0" t="s">
-        <v>141</v>
-      </c>
-      <c r="D32" s="0" t="s">
-        <v>142</v>
-      </c>
-      <c r="E32" s="0" t="n">
-        <v>35</v>
-      </c>
-      <c r="F32" s="0" t="n">
-        <v>36</v>
-      </c>
-      <c r="G32" s="0" t="n">
+      <c r="H32" s="0" t="n">
         <v>3.12</v>
       </c>
-      <c r="H32" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="I32" s="0" t="s">
-        <v>143</v>
+      <c r="I32" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="J32" s="0" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>144</v>
+        <v>118</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>145</v>
+        <v>119</v>
       </c>
       <c r="C33" s="0" t="s">
-        <v>146</v>
+        <v>120</v>
       </c>
       <c r="D33" s="0" t="s">
-        <v>147</v>
+        <v>38</v>
       </c>
       <c r="E33" s="0" t="n">
+        <v>1775</v>
+      </c>
+      <c r="F33" s="0" t="n">
         <v>35</v>
       </c>
-      <c r="F33" s="0" t="n">
+      <c r="G33" s="0" t="n">
         <v>37</v>
       </c>
-      <c r="G33" s="0" t="n">
+      <c r="H33" s="0" t="n">
         <v>3.12</v>
       </c>
-      <c r="H33" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="I33" s="0" t="s">
-        <v>148</v>
+      <c r="I33" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="J33" s="0" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>149</v>
+        <v>122</v>
       </c>
       <c r="B34" s="0" t="s">
         <v>16</v>
       </c>
       <c r="C34" s="0" t="s">
-        <v>150</v>
-      </c>
-      <c r="D34" s="0" t="s">
-        <v>151</v>
+        <v>123</v>
+      </c>
+      <c r="D34" s="0" t="n">
+        <v>18119</v>
       </c>
       <c r="E34" s="0" t="n">
+        <v>769</v>
+      </c>
+      <c r="F34" s="0" t="n">
         <v>29</v>
       </c>
-      <c r="F34" s="0" t="n">
+      <c r="G34" s="0" t="n">
         <v>26</v>
       </c>
-      <c r="G34" s="0" t="n">
+      <c r="H34" s="0" t="n">
         <v>3.12</v>
       </c>
-      <c r="H34" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="I34" s="0" t="s">
-        <v>153</v>
+      <c r="I34" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="J34" s="0" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>154</v>
+        <v>126</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C35" s="0" t="s">
-        <v>155</v>
-      </c>
-      <c r="D35" s="0" t="s">
-        <v>156</v>
+        <v>127</v>
+      </c>
+      <c r="D35" s="0" t="n">
+        <v>27639</v>
       </c>
       <c r="E35" s="0" t="n">
+        <v>1745</v>
+      </c>
+      <c r="F35" s="0" t="n">
         <v>35</v>
       </c>
-      <c r="F35" s="0" t="n">
+      <c r="G35" s="0" t="n">
         <v>37</v>
       </c>
-      <c r="G35" s="0" t="n">
+      <c r="H35" s="0" t="n">
         <v>3.12</v>
       </c>
-      <c r="H35" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="I35" s="0" t="s">
-        <v>157</v>
+      <c r="I35" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="J35" s="0" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>158</v>
+        <v>129</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C36" s="0" t="s">
-        <v>159</v>
-      </c>
-      <c r="D36" s="0" t="s">
-        <v>160</v>
+        <v>130</v>
+      </c>
+      <c r="D36" s="0" t="n">
+        <v>19144</v>
       </c>
       <c r="E36" s="0" t="n">
+        <v>1304</v>
+      </c>
+      <c r="F36" s="0" t="n">
         <v>35</v>
       </c>
-      <c r="F36" s="0" t="n">
+      <c r="G36" s="0" t="n">
         <v>37</v>
       </c>
-      <c r="G36" s="0" t="n">
+      <c r="H36" s="0" t="n">
         <v>3.12</v>
       </c>
-      <c r="H36" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="I36" s="0" t="s">
-        <v>161</v>
+      <c r="I36" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="J36" s="0" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>162</v>
+        <v>132</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>163</v>
+        <v>133</v>
       </c>
       <c r="C37" s="0" t="s">
-        <v>164</v>
-      </c>
-      <c r="D37" s="0" t="s">
-        <v>165</v>
+        <v>134</v>
+      </c>
+      <c r="D37" s="0" t="n">
+        <v>18802</v>
       </c>
       <c r="E37" s="0" t="n">
+        <v>1741</v>
+      </c>
+      <c r="F37" s="0" t="n">
         <v>32</v>
       </c>
-      <c r="F37" s="0" t="n">
+      <c r="G37" s="0" t="n">
         <v>34</v>
       </c>
-      <c r="G37" s="0" t="n">
+      <c r="H37" s="0" t="n">
         <v>3.12</v>
       </c>
-      <c r="H37" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="I37" s="0" t="s">
-        <v>166</v>
+      <c r="I37" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="J37" s="0" t="s">
+        <v>135</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>167</v>
+        <v>136</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>168</v>
+        <v>137</v>
       </c>
       <c r="C38" s="0" t="s">
-        <v>169</v>
+        <v>138</v>
       </c>
       <c r="D38" s="0" t="s">
-        <v>170</v>
+        <v>38</v>
       </c>
       <c r="E38" s="0" t="n">
+        <v>1804</v>
+      </c>
+      <c r="F38" s="0" t="n">
         <v>35</v>
       </c>
-      <c r="F38" s="0" t="n">
-        <v>38</v>
-      </c>
       <c r="G38" s="0" t="n">
+        <v>38</v>
+      </c>
+      <c r="H38" s="0" t="n">
         <v>3.12</v>
       </c>
-      <c r="H38" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="I38" s="0" t="s">
-        <v>171</v>
+      <c r="I38" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="J38" s="0" t="s">
+        <v>139</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>172</v>
+        <v>140</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>173</v>
+        <v>141</v>
       </c>
       <c r="C39" s="0" t="s">
-        <v>174</v>
-      </c>
-      <c r="D39" s="0" t="s">
-        <v>175</v>
+        <v>142</v>
+      </c>
+      <c r="D39" s="0" t="n">
+        <v>12399</v>
       </c>
       <c r="E39" s="0" t="n">
+        <v>375</v>
+      </c>
+      <c r="F39" s="0" t="n">
         <v>24</v>
       </c>
-      <c r="F39" s="0" t="n">
+      <c r="G39" s="0" t="n">
         <v>27</v>
       </c>
-      <c r="G39" s="0" t="n">
+      <c r="H39" s="0" t="n">
         <v>3.12</v>
       </c>
-      <c r="H39" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="I39" s="0" t="s">
-        <v>176</v>
+      <c r="I39" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="J39" s="0" t="s">
+        <v>143</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>177</v>
+        <v>144</v>
       </c>
       <c r="B40" s="0" t="s">
         <v>16</v>
       </c>
       <c r="C40" s="0" t="s">
-        <v>178</v>
-      </c>
-      <c r="D40" s="0" t="s">
-        <v>151</v>
+        <v>145</v>
+      </c>
+      <c r="D40" s="0" t="n">
+        <v>18119</v>
       </c>
       <c r="E40" s="0" t="n">
+        <v>769</v>
+      </c>
+      <c r="F40" s="0" t="n">
         <v>29</v>
       </c>
-      <c r="F40" s="0" t="n">
+      <c r="G40" s="0" t="n">
         <v>26</v>
       </c>
-      <c r="G40" s="0" t="n">
+      <c r="H40" s="0" t="n">
         <v>3.12</v>
       </c>
-      <c r="H40" s="1" t="s">
-        <v>179</v>
-      </c>
-      <c r="I40" s="0" t="s">
-        <v>180</v>
+      <c r="I40" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="J40" s="0" t="s">
+        <v>147</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>181</v>
+        <v>148</v>
       </c>
       <c r="B41" s="0" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C41" s="0" t="s">
-        <v>182</v>
-      </c>
-      <c r="D41" s="0" t="s">
-        <v>156</v>
+        <v>149</v>
+      </c>
+      <c r="D41" s="0" t="n">
+        <v>27639</v>
       </c>
       <c r="E41" s="0" t="n">
+        <v>1745</v>
+      </c>
+      <c r="F41" s="0" t="n">
         <v>35</v>
       </c>
-      <c r="F41" s="0" t="n">
+      <c r="G41" s="0" t="n">
         <v>37</v>
       </c>
-      <c r="G41" s="0" t="n">
+      <c r="H41" s="0" t="n">
         <v>3.12</v>
       </c>
-      <c r="H41" s="1" t="s">
-        <v>179</v>
-      </c>
-      <c r="I41" s="0" t="s">
-        <v>183</v>
+      <c r="I41" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="J41" s="0" t="s">
+        <v>150</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>184</v>
+        <v>151</v>
       </c>
       <c r="B42" s="0" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C42" s="0" t="s">
-        <v>185</v>
-      </c>
-      <c r="D42" s="0" t="s">
-        <v>160</v>
+        <v>152</v>
+      </c>
+      <c r="D42" s="0" t="n">
+        <v>19144</v>
       </c>
       <c r="E42" s="0" t="n">
+        <v>1304</v>
+      </c>
+      <c r="F42" s="0" t="n">
         <v>32</v>
       </c>
-      <c r="F42" s="0" t="n">
+      <c r="G42" s="0" t="n">
         <v>34</v>
       </c>
-      <c r="G42" s="0" t="n">
+      <c r="H42" s="0" t="n">
         <v>3.12</v>
       </c>
-      <c r="H42" s="1" t="s">
-        <v>179</v>
-      </c>
-      <c r="I42" s="0" t="s">
-        <v>186</v>
+      <c r="I42" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="J42" s="0" t="s">
+        <v>153</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>187</v>
+        <v>154</v>
       </c>
       <c r="B43" s="0" t="s">
-        <v>163</v>
+        <v>133</v>
       </c>
       <c r="C43" s="0" t="s">
-        <v>188</v>
-      </c>
-      <c r="D43" s="0" t="s">
-        <v>165</v>
+        <v>155</v>
+      </c>
+      <c r="D43" s="0" t="n">
+        <v>18802</v>
       </c>
       <c r="E43" s="0" t="n">
+        <v>1741</v>
+      </c>
+      <c r="F43" s="0" t="n">
         <v>35</v>
       </c>
-      <c r="F43" s="0" t="n">
+      <c r="G43" s="0" t="n">
         <v>37</v>
       </c>
-      <c r="G43" s="0" t="n">
+      <c r="H43" s="0" t="n">
         <v>3.12</v>
       </c>
-      <c r="H43" s="1" t="s">
-        <v>179</v>
-      </c>
-      <c r="I43" s="0" t="s">
-        <v>189</v>
+      <c r="I43" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="J43" s="0" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
-        <v>190</v>
+        <v>157</v>
       </c>
       <c r="B44" s="0" t="s">
-        <v>191</v>
+        <v>158</v>
       </c>
       <c r="C44" s="0" t="s">
-        <v>192</v>
+        <v>159</v>
       </c>
       <c r="D44" s="0" t="s">
-        <v>170</v>
+        <v>38</v>
       </c>
       <c r="E44" s="0" t="n">
+        <v>1804</v>
+      </c>
+      <c r="F44" s="0" t="n">
         <v>35</v>
       </c>
-      <c r="F44" s="0" t="n">
-        <v>38</v>
-      </c>
       <c r="G44" s="0" t="n">
+        <v>38</v>
+      </c>
+      <c r="H44" s="0" t="n">
         <v>3.12</v>
       </c>
-      <c r="H44" s="1" t="s">
-        <v>179</v>
-      </c>
-      <c r="I44" s="0" t="s">
-        <v>193</v>
+      <c r="I44" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="J44" s="0" t="s">
+        <v>160</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>194</v>
+        <v>161</v>
       </c>
       <c r="B45" s="0" t="s">
         <v>16</v>
       </c>
       <c r="C45" s="0" t="s">
-        <v>195</v>
-      </c>
-      <c r="D45" s="0" t="s">
-        <v>196</v>
+        <v>162</v>
+      </c>
+      <c r="D45" s="0" t="n">
+        <v>18119</v>
       </c>
       <c r="E45" s="0" t="n">
+        <v>808</v>
+      </c>
+      <c r="F45" s="0" t="n">
         <v>31</v>
       </c>
-      <c r="F45" s="0" t="n">
+      <c r="G45" s="0" t="n">
         <v>29</v>
       </c>
-      <c r="G45" s="0" t="n">
+      <c r="H45" s="0" t="n">
         <v>3.12</v>
       </c>
-      <c r="H45" s="1" t="s">
-        <v>197</v>
-      </c>
-      <c r="I45" s="0" t="s">
-        <v>198</v>
+      <c r="I45" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="J45" s="0" t="s">
+        <v>164</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
-        <v>199</v>
+        <v>165</v>
       </c>
       <c r="B46" s="0" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C46" s="0" t="s">
-        <v>200</v>
-      </c>
-      <c r="D46" s="0" t="s">
-        <v>201</v>
+        <v>166</v>
+      </c>
+      <c r="D46" s="0" t="n">
+        <v>27562</v>
       </c>
       <c r="E46" s="0" t="n">
+        <v>1753</v>
+      </c>
+      <c r="F46" s="0" t="n">
         <v>35</v>
       </c>
-      <c r="F46" s="0" t="n">
-        <v>38</v>
-      </c>
       <c r="G46" s="0" t="n">
+        <v>38</v>
+      </c>
+      <c r="H46" s="0" t="n">
         <v>3.12</v>
       </c>
-      <c r="H46" s="1" t="s">
-        <v>197</v>
-      </c>
-      <c r="I46" s="0" t="s">
-        <v>202</v>
+      <c r="I46" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="J46" s="0" t="s">
+        <v>167</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
-        <v>203</v>
+        <v>168</v>
       </c>
       <c r="B47" s="0" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C47" s="0" t="s">
-        <v>204</v>
-      </c>
-      <c r="D47" s="0" t="s">
-        <v>205</v>
+        <v>169</v>
+      </c>
+      <c r="D47" s="0" t="n">
+        <v>19182</v>
       </c>
       <c r="E47" s="0" t="n">
+        <v>1376</v>
+      </c>
+      <c r="F47" s="0" t="n">
         <v>33</v>
       </c>
-      <c r="F47" s="0" t="n">
+      <c r="G47" s="0" t="n">
         <v>37</v>
       </c>
-      <c r="G47" s="0" t="n">
+      <c r="H47" s="0" t="n">
         <v>3.12</v>
       </c>
-      <c r="H47" s="1" t="s">
-        <v>197</v>
-      </c>
-      <c r="I47" s="0" t="s">
-        <v>206</v>
+      <c r="I47" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="J47" s="0" t="s">
+        <v>170</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
-        <v>207</v>
+        <v>171</v>
       </c>
       <c r="B48" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="C48" s="0" t="s">
+        <v>172</v>
+      </c>
+      <c r="D48" s="0" t="n">
+        <v>18789</v>
+      </c>
+      <c r="E48" s="0" t="n">
+        <v>1749</v>
+      </c>
+      <c r="F48" s="0" t="n">
+        <v>35</v>
+      </c>
+      <c r="G48" s="0" t="n">
+        <v>38</v>
+      </c>
+      <c r="H48" s="0" t="n">
+        <v>3.12</v>
+      </c>
+      <c r="I48" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="C48" s="0" t="s">
-        <v>208</v>
-      </c>
-      <c r="D48" s="0" t="s">
-        <v>209</v>
-      </c>
-      <c r="E48" s="0" t="n">
-        <v>35</v>
-      </c>
-      <c r="F48" s="0" t="n">
-        <v>38</v>
-      </c>
-      <c r="G48" s="0" t="n">
-        <v>3.12</v>
-      </c>
-      <c r="H48" s="1" t="s">
-        <v>197</v>
-      </c>
-      <c r="I48" s="0" t="s">
-        <v>210</v>
+      <c r="J48" s="0" t="s">
+        <v>173</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
-        <v>211</v>
+        <v>174</v>
       </c>
       <c r="B49" s="0" t="s">
-        <v>212</v>
+        <v>175</v>
       </c>
       <c r="C49" s="0" t="s">
-        <v>213</v>
+        <v>176</v>
       </c>
       <c r="D49" s="0" t="s">
-        <v>214</v>
+        <v>38</v>
       </c>
       <c r="E49" s="0" t="n">
+        <v>1812</v>
+      </c>
+      <c r="F49" s="0" t="n">
         <v>35</v>
       </c>
-      <c r="F49" s="0" t="n">
+      <c r="G49" s="0" t="n">
         <v>39</v>
       </c>
-      <c r="G49" s="0" t="n">
+      <c r="H49" s="0" t="n">
         <v>3.12</v>
       </c>
-      <c r="H49" s="1" t="s">
-        <v>197</v>
-      </c>
-      <c r="I49" s="0" t="s">
-        <v>215</v>
+      <c r="I49" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="J49" s="0" t="s">
+        <v>177</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
-        <v>216</v>
+        <v>178</v>
       </c>
       <c r="B50" s="0" t="s">
         <v>16</v>
       </c>
       <c r="C50" s="0" t="s">
-        <v>217</v>
-      </c>
-      <c r="D50" s="0" t="s">
-        <v>196</v>
+        <v>179</v>
+      </c>
+      <c r="D50" s="0" t="n">
+        <v>18119</v>
       </c>
       <c r="E50" s="0" t="n">
+        <v>808</v>
+      </c>
+      <c r="F50" s="0" t="n">
         <v>31</v>
       </c>
-      <c r="F50" s="0" t="n">
+      <c r="G50" s="0" t="n">
         <v>29</v>
       </c>
-      <c r="G50" s="0" t="n">
+      <c r="H50" s="0" t="n">
         <v>3.12</v>
       </c>
-      <c r="H50" s="1" t="s">
-        <v>218</v>
-      </c>
-      <c r="I50" s="0" t="s">
-        <v>219</v>
+      <c r="I50" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="J50" s="0" t="s">
+        <v>181</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
-        <v>220</v>
+        <v>182</v>
       </c>
       <c r="B51" s="0" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C51" s="0" t="s">
-        <v>221</v>
-      </c>
-      <c r="D51" s="0" t="s">
-        <v>222</v>
+        <v>183</v>
+      </c>
+      <c r="D51" s="0" t="n">
+        <v>27562</v>
       </c>
       <c r="E51" s="0" t="n">
+        <v>1740</v>
+      </c>
+      <c r="F51" s="0" t="n">
         <v>35</v>
       </c>
-      <c r="F51" s="0" t="n">
-        <v>38</v>
-      </c>
       <c r="G51" s="0" t="n">
+        <v>38</v>
+      </c>
+      <c r="H51" s="0" t="n">
         <v>3.12</v>
       </c>
-      <c r="H51" s="1" t="s">
-        <v>218</v>
-      </c>
-      <c r="I51" s="0" t="s">
-        <v>223</v>
+      <c r="I51" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="J51" s="0" t="s">
+        <v>184</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
-        <v>224</v>
+        <v>185</v>
       </c>
       <c r="B52" s="0" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C52" s="0" t="s">
-        <v>225</v>
-      </c>
-      <c r="D52" s="0" t="s">
-        <v>226</v>
+        <v>186</v>
+      </c>
+      <c r="D52" s="0" t="n">
+        <v>19177</v>
       </c>
       <c r="E52" s="0" t="n">
+        <v>1376</v>
+      </c>
+      <c r="F52" s="0" t="n">
         <v>33</v>
       </c>
-      <c r="F52" s="0" t="n">
+      <c r="G52" s="0" t="n">
         <v>37</v>
       </c>
-      <c r="G52" s="0" t="n">
+      <c r="H52" s="0" t="n">
         <v>3.12</v>
       </c>
-      <c r="H52" s="1" t="s">
-        <v>218</v>
-      </c>
-      <c r="I52" s="0" t="s">
-        <v>227</v>
+      <c r="I52" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="J52" s="0" t="s">
+        <v>187</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="s">
-        <v>228</v>
+        <v>188</v>
       </c>
       <c r="B53" s="0" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C53" s="0" t="s">
-        <v>229</v>
-      </c>
-      <c r="D53" s="0" t="s">
-        <v>230</v>
+        <v>189</v>
+      </c>
+      <c r="D53" s="0" t="n">
+        <v>18788</v>
       </c>
       <c r="E53" s="0" t="n">
+        <v>1747</v>
+      </c>
+      <c r="F53" s="0" t="n">
         <v>35</v>
       </c>
-      <c r="F53" s="0" t="n">
-        <v>38</v>
-      </c>
       <c r="G53" s="0" t="n">
+        <v>38</v>
+      </c>
+      <c r="H53" s="0" t="n">
         <v>3.12</v>
       </c>
-      <c r="H53" s="1" t="s">
-        <v>218</v>
-      </c>
-      <c r="I53" s="0" t="s">
-        <v>231</v>
+      <c r="I53" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="J53" s="0" t="s">
+        <v>190</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="s">
-        <v>232</v>
+        <v>191</v>
       </c>
       <c r="B54" s="0" t="s">
-        <v>233</v>
+        <v>192</v>
       </c>
       <c r="C54" s="0" t="s">
-        <v>234</v>
+        <v>193</v>
       </c>
       <c r="D54" s="0" t="s">
-        <v>235</v>
+        <v>38</v>
       </c>
       <c r="E54" s="0" t="n">
+        <v>1811</v>
+      </c>
+      <c r="F54" s="0" t="n">
         <v>35</v>
       </c>
-      <c r="F54" s="0" t="n">
+      <c r="G54" s="0" t="n">
         <v>39</v>
       </c>
-      <c r="G54" s="0" t="n">
+      <c r="H54" s="0" t="n">
         <v>3.12</v>
       </c>
-      <c r="H54" s="1" t="s">
-        <v>218</v>
-      </c>
-      <c r="I54" s="0" t="s">
-        <v>236</v>
+      <c r="I54" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="J54" s="0" t="s">
+        <v>194</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
-        <v>237</v>
+        <v>195</v>
       </c>
       <c r="B55" s="0" t="s">
         <v>16</v>
       </c>
       <c r="C55" s="0" t="s">
-        <v>238</v>
-      </c>
-      <c r="D55" s="0" t="s">
-        <v>239</v>
+        <v>196</v>
+      </c>
+      <c r="D55" s="0" t="n">
+        <v>17645</v>
       </c>
       <c r="E55" s="0" t="n">
+        <v>990</v>
+      </c>
+      <c r="F55" s="0" t="n">
         <v>32</v>
       </c>
-      <c r="F55" s="0" t="n">
+      <c r="G55" s="0" t="n">
         <v>30</v>
       </c>
-      <c r="G55" s="0" t="n">
+      <c r="H55" s="0" t="n">
         <v>3.13</v>
       </c>
-      <c r="H55" s="1" t="s">
-        <v>240</v>
-      </c>
-      <c r="I55" s="0" t="s">
-        <v>241</v>
+      <c r="I55" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="J55" s="0" t="s">
+        <v>198</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
-        <v>242</v>
+        <v>199</v>
       </c>
       <c r="B56" s="0" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C56" s="0" t="s">
-        <v>243</v>
-      </c>
-      <c r="D56" s="0" t="s">
-        <v>244</v>
+        <v>200</v>
+      </c>
+      <c r="D56" s="0" t="n">
+        <v>27562</v>
       </c>
       <c r="E56" s="0" t="n">
+        <v>1742</v>
+      </c>
+      <c r="F56" s="0" t="n">
         <v>35</v>
       </c>
-      <c r="F56" s="0" t="n">
-        <v>38</v>
-      </c>
       <c r="G56" s="0" t="n">
+        <v>38</v>
+      </c>
+      <c r="H56" s="0" t="n">
         <v>3.13</v>
       </c>
-      <c r="H56" s="1" t="s">
-        <v>240</v>
-      </c>
-      <c r="I56" s="0" t="s">
-        <v>245</v>
+      <c r="I56" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="J56" s="0" t="s">
+        <v>201</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="s">
-        <v>246</v>
+        <v>202</v>
       </c>
       <c r="B57" s="0" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C57" s="0" t="s">
-        <v>247</v>
-      </c>
-      <c r="D57" s="0" t="s">
-        <v>248</v>
+        <v>203</v>
+      </c>
+      <c r="D57" s="0" t="n">
+        <v>19177</v>
       </c>
       <c r="E57" s="0" t="n">
+        <v>1379</v>
+      </c>
+      <c r="F57" s="0" t="n">
         <v>33</v>
       </c>
-      <c r="F57" s="0" t="n">
+      <c r="G57" s="0" t="n">
         <v>37</v>
       </c>
-      <c r="G57" s="0" t="n">
+      <c r="H57" s="0" t="n">
         <v>3.13</v>
       </c>
-      <c r="H57" s="1" t="s">
-        <v>240</v>
-      </c>
-      <c r="I57" s="0" t="s">
-        <v>249</v>
+      <c r="I57" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="J57" s="0" t="s">
+        <v>204</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="s">
-        <v>250</v>
+        <v>205</v>
       </c>
       <c r="B58" s="0" t="s">
-        <v>163</v>
+        <v>133</v>
       </c>
       <c r="C58" s="0" t="s">
-        <v>251</v>
-      </c>
-      <c r="D58" s="0" t="s">
-        <v>252</v>
+        <v>206</v>
+      </c>
+      <c r="D58" s="0" t="n">
+        <v>18787</v>
       </c>
       <c r="E58" s="0" t="n">
+        <v>1750</v>
+      </c>
+      <c r="F58" s="0" t="n">
         <v>35</v>
       </c>
-      <c r="F58" s="0" t="n">
-        <v>38</v>
-      </c>
       <c r="G58" s="0" t="n">
+        <v>38</v>
+      </c>
+      <c r="H58" s="0" t="n">
         <v>3.13</v>
       </c>
-      <c r="H58" s="1" t="s">
-        <v>240</v>
-      </c>
-      <c r="I58" s="0" t="s">
-        <v>253</v>
+      <c r="I58" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="J58" s="0" t="s">
+        <v>207</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="s">
-        <v>254</v>
+        <v>208</v>
       </c>
       <c r="B59" s="0" t="s">
-        <v>255</v>
+        <v>209</v>
       </c>
       <c r="C59" s="0" t="s">
-        <v>256</v>
+        <v>210</v>
       </c>
       <c r="D59" s="0" t="s">
-        <v>257</v>
+        <v>38</v>
       </c>
       <c r="E59" s="0" t="n">
+        <v>1814</v>
+      </c>
+      <c r="F59" s="0" t="n">
         <v>35</v>
       </c>
-      <c r="F59" s="0" t="n">
+      <c r="G59" s="0" t="n">
         <v>39</v>
       </c>
-      <c r="G59" s="0" t="n">
+      <c r="H59" s="0" t="n">
         <v>3.13</v>
       </c>
-      <c r="H59" s="1" t="s">
-        <v>240</v>
-      </c>
-      <c r="I59" s="0" t="s">
-        <v>258</v>
+      <c r="I59" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="J59" s="0" t="s">
+        <v>211</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="s">
-        <v>259</v>
+        <v>212</v>
       </c>
       <c r="B60" s="0" t="s">
-        <v>260</v>
-      </c>
-      <c r="C60" s="2" t="s">
-        <v>261</v>
-      </c>
-      <c r="D60" s="0" t="s">
-        <v>262</v>
+        <v>213</v>
+      </c>
+      <c r="C60" s="3" t="s">
+        <v>214</v>
+      </c>
+      <c r="D60" s="0" t="n">
+        <v>17393</v>
       </c>
       <c r="E60" s="0" t="n">
+        <v>1032</v>
+      </c>
+      <c r="F60" s="0" t="n">
         <v>32</v>
       </c>
-      <c r="F60" s="0" t="n">
+      <c r="G60" s="0" t="n">
         <v>30</v>
       </c>
-      <c r="G60" s="0" t="n">
+      <c r="H60" s="0" t="n">
         <v>3.14</v>
       </c>
-      <c r="H60" s="1" t="s">
-        <v>263</v>
-      </c>
-      <c r="I60" s="0" t="s">
-        <v>264</v>
+      <c r="I60" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="J60" s="0" t="s">
+        <v>216</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="s">
-        <v>265</v>
+        <v>217</v>
       </c>
       <c r="B61" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="C61" s="2" t="s">
-        <v>266</v>
-      </c>
-      <c r="D61" s="0" t="s">
-        <v>267</v>
+        <v>20</v>
+      </c>
+      <c r="C61" s="3" t="s">
+        <v>218</v>
+      </c>
+      <c r="D61" s="0" t="n">
+        <v>27562</v>
       </c>
       <c r="E61" s="0" t="n">
+        <v>1741</v>
+      </c>
+      <c r="F61" s="0" t="n">
         <v>35</v>
       </c>
-      <c r="F61" s="0" t="n">
+      <c r="G61" s="0" t="n">
         <v>37</v>
       </c>
-      <c r="G61" s="0" t="n">
+      <c r="H61" s="0" t="n">
         <v>3.14</v>
       </c>
-      <c r="H61" s="1" t="s">
-        <v>263</v>
-      </c>
-      <c r="I61" s="0" t="s">
-        <v>268</v>
+      <c r="I61" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="J61" s="0" t="s">
+        <v>219</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="s">
-        <v>269</v>
+        <v>220</v>
       </c>
       <c r="B62" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="C62" s="2" t="s">
-        <v>270</v>
-      </c>
-      <c r="D62" s="0" t="s">
-        <v>271</v>
+        <v>28</v>
+      </c>
+      <c r="C62" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="D62" s="0" t="n">
+        <v>19177</v>
       </c>
       <c r="E62" s="0" t="n">
+        <v>1377</v>
+      </c>
+      <c r="F62" s="0" t="n">
         <v>33</v>
       </c>
-      <c r="F62" s="0" t="n">
+      <c r="G62" s="0" t="n">
         <v>37</v>
       </c>
-      <c r="G62" s="0" t="n">
+      <c r="H62" s="0" t="n">
         <v>3.14</v>
       </c>
-      <c r="H62" s="1" t="s">
-        <v>263</v>
-      </c>
-      <c r="I62" s="0" t="s">
-        <v>272</v>
+      <c r="I62" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="J62" s="0" t="s">
+        <v>222</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="s">
-        <v>273</v>
+        <v>223</v>
       </c>
       <c r="B63" s="0" t="s">
-        <v>163</v>
-      </c>
-      <c r="C63" s="2" t="s">
-        <v>274</v>
-      </c>
-      <c r="D63" s="0" t="s">
-        <v>275</v>
+        <v>133</v>
+      </c>
+      <c r="C63" s="3" t="s">
+        <v>224</v>
+      </c>
+      <c r="D63" s="0" t="n">
+        <v>18784</v>
       </c>
       <c r="E63" s="0" t="n">
+        <v>1746</v>
+      </c>
+      <c r="F63" s="0" t="n">
         <v>35</v>
       </c>
-      <c r="F63" s="0" t="n">
+      <c r="G63" s="0" t="n">
         <v>37</v>
       </c>
-      <c r="G63" s="0" t="n">
+      <c r="H63" s="0" t="n">
         <v>3.14</v>
       </c>
-      <c r="H63" s="1" t="s">
-        <v>263</v>
-      </c>
-      <c r="I63" s="0" t="s">
-        <v>276</v>
+      <c r="I63" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="J63" s="0" t="s">
+        <v>225</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="s">
-        <v>277</v>
+        <v>226</v>
       </c>
       <c r="B64" s="0" t="s">
-        <v>278</v>
-      </c>
-      <c r="C64" s="2" t="s">
-        <v>279</v>
+        <v>227</v>
+      </c>
+      <c r="C64" s="3" t="s">
+        <v>228</v>
       </c>
       <c r="D64" s="0" t="s">
-        <v>280</v>
+        <v>38</v>
       </c>
       <c r="E64" s="0" t="n">
+        <v>2944</v>
+      </c>
+      <c r="F64" s="0" t="n">
         <v>43</v>
       </c>
-      <c r="F64" s="0" t="n">
+      <c r="G64" s="0" t="n">
         <v>47</v>
       </c>
-      <c r="G64" s="0" t="n">
+      <c r="H64" s="0" t="n">
         <v>3.14</v>
       </c>
-      <c r="H64" s="1" t="s">
-        <v>263</v>
-      </c>
-      <c r="I64" s="0" t="s">
-        <v>281</v>
+      <c r="I64" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="J64" s="0" t="s">
+        <v>229</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="0" t="s">
-        <v>282</v>
+        <v>230</v>
       </c>
       <c r="B65" s="0" t="s">
-        <v>260</v>
+        <v>213</v>
       </c>
       <c r="C65" s="0" t="s">
-        <v>283</v>
-      </c>
-      <c r="D65" s="0" t="s">
-        <v>284</v>
+        <v>231</v>
+      </c>
+      <c r="D65" s="0" t="n">
+        <v>17386</v>
       </c>
       <c r="E65" s="0" t="n">
+        <v>1032</v>
+      </c>
+      <c r="F65" s="0" t="n">
         <v>32</v>
       </c>
-      <c r="F65" s="0" t="n">
+      <c r="G65" s="0" t="n">
         <v>30</v>
       </c>
-      <c r="G65" s="0" t="n">
+      <c r="H65" s="0" t="n">
         <v>3.14</v>
       </c>
-      <c r="H65" s="1" t="s">
-        <v>285</v>
-      </c>
-      <c r="I65" s="0" t="s">
-        <v>286</v>
+      <c r="I65" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="J65" s="0" t="s">
+        <v>233</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="0" t="s">
-        <v>287</v>
+        <v>234</v>
       </c>
       <c r="B66" s="0" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C66" s="0" t="s">
-        <v>288</v>
-      </c>
-      <c r="D66" s="0" t="s">
-        <v>289</v>
+        <v>235</v>
+      </c>
+      <c r="D66" s="0" t="n">
+        <v>25368</v>
       </c>
       <c r="E66" s="0" t="n">
+        <v>1750</v>
+      </c>
+      <c r="F66" s="0" t="n">
         <v>35</v>
       </c>
-      <c r="F66" s="0" t="n">
+      <c r="G66" s="0" t="n">
         <v>37</v>
       </c>
-      <c r="G66" s="0" t="n">
+      <c r="H66" s="0" t="n">
         <v>3.14</v>
       </c>
-      <c r="H66" s="1" t="s">
-        <v>285</v>
-      </c>
-      <c r="I66" s="0" t="s">
-        <v>290</v>
+      <c r="I66" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="J66" s="0" t="s">
+        <v>236</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="0" t="s">
-        <v>291</v>
+        <v>237</v>
       </c>
       <c r="B67" s="0" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C67" s="0" t="s">
-        <v>292</v>
-      </c>
-      <c r="D67" s="0" t="s">
-        <v>293</v>
+        <v>238</v>
+      </c>
+      <c r="D67" s="0" t="n">
+        <v>19177</v>
       </c>
       <c r="E67" s="0" t="n">
+        <v>1389</v>
+      </c>
+      <c r="F67" s="0" t="n">
         <v>33</v>
       </c>
-      <c r="F67" s="0" t="n">
+      <c r="G67" s="0" t="n">
         <v>37</v>
       </c>
-      <c r="G67" s="0" t="n">
+      <c r="H67" s="0" t="n">
         <v>3.14</v>
       </c>
-      <c r="H67" s="1" t="s">
-        <v>285</v>
-      </c>
-      <c r="I67" s="0" t="s">
-        <v>294</v>
+      <c r="I67" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="J67" s="0" t="s">
+        <v>239</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="0" t="s">
-        <v>295</v>
+        <v>240</v>
       </c>
       <c r="B68" s="0" t="s">
-        <v>163</v>
+        <v>133</v>
       </c>
       <c r="C68" s="0" t="s">
-        <v>296</v>
-      </c>
-      <c r="D68" s="0" t="s">
-        <v>297</v>
+        <v>241</v>
+      </c>
+      <c r="D68" s="0" t="n">
+        <v>18784</v>
       </c>
       <c r="E68" s="0" t="n">
+        <v>1755</v>
+      </c>
+      <c r="F68" s="0" t="n">
         <v>35</v>
       </c>
-      <c r="F68" s="0" t="n">
+      <c r="G68" s="0" t="n">
         <v>37</v>
       </c>
-      <c r="G68" s="0" t="n">
+      <c r="H68" s="0" t="n">
         <v>3.14</v>
       </c>
-      <c r="H68" s="1" t="s">
-        <v>285</v>
-      </c>
-      <c r="I68" s="0" t="s">
-        <v>298</v>
+      <c r="I68" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="J68" s="0" t="s">
+        <v>242</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="0" t="s">
-        <v>299</v>
+        <v>243</v>
       </c>
       <c r="B69" s="0" t="s">
-        <v>300</v>
+        <v>244</v>
       </c>
       <c r="C69" s="0" t="s">
-        <v>301</v>
+        <v>245</v>
       </c>
       <c r="D69" s="0" t="s">
-        <v>302</v>
+        <v>38</v>
       </c>
       <c r="E69" s="0" t="n">
+        <v>1825</v>
+      </c>
+      <c r="F69" s="0" t="n">
         <v>35</v>
       </c>
-      <c r="F69" s="0" t="n">
+      <c r="G69" s="0" t="n">
         <v>39</v>
       </c>
-      <c r="G69" s="0" t="n">
+      <c r="H69" s="0" t="n">
         <v>3.14</v>
       </c>
-      <c r="H69" s="1" t="s">
-        <v>285</v>
-      </c>
-      <c r="I69" s="0" t="s">
-        <v>303</v>
+      <c r="I69" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="J69" s="0" t="s">
+        <v>246</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="0" t="s">
-        <v>304</v>
+        <v>247</v>
       </c>
       <c r="B70" s="0" t="s">
-        <v>260</v>
-      </c>
-      <c r="D70" s="0" t="s">
-        <v>305</v>
+        <v>213</v>
+      </c>
+      <c r="C70" s="0" t="s">
+        <v>248</v>
+      </c>
+      <c r="D70" s="0" t="n">
+        <v>17386</v>
       </c>
       <c r="E70" s="0" t="n">
+        <v>1070</v>
+      </c>
+      <c r="F70" s="0" t="n">
         <v>32</v>
       </c>
-      <c r="F70" s="0" t="n">
+      <c r="G70" s="0" t="n">
         <v>31</v>
       </c>
-      <c r="G70" s="0" t="n">
+      <c r="H70" s="0" t="n">
         <v>3.15</v>
       </c>
-      <c r="H70" s="1" t="s">
-        <v>306</v>
-      </c>
-      <c r="I70" s="0" t="s">
-        <v>307</v>
+      <c r="I70" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="J70" s="0" t="s">
+        <v>250</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="0" t="s">
-        <v>308</v>
+        <v>251</v>
       </c>
       <c r="B71" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="D71" s="0" t="s">
-        <v>309</v>
+        <v>20</v>
+      </c>
+      <c r="C71" s="0" t="s">
+        <v>252</v>
+      </c>
+      <c r="D71" s="0" t="n">
+        <v>25368</v>
       </c>
       <c r="E71" s="0" t="n">
+        <v>1754</v>
+      </c>
+      <c r="F71" s="0" t="n">
         <v>35</v>
       </c>
-      <c r="F71" s="0" t="n">
-        <v>38</v>
-      </c>
       <c r="G71" s="0" t="n">
+        <v>38</v>
+      </c>
+      <c r="H71" s="0" t="n">
         <v>3.15</v>
       </c>
-      <c r="H71" s="1" t="s">
-        <v>306</v>
-      </c>
-      <c r="I71" s="0" t="s">
-        <v>310</v>
+      <c r="I71" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="J71" s="0" t="s">
+        <v>253</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="0" t="s">
-        <v>311</v>
+        <v>254</v>
       </c>
       <c r="B72" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="D72" s="0" t="s">
-        <v>312</v>
+        <v>28</v>
+      </c>
+      <c r="C72" s="0" t="s">
+        <v>255</v>
+      </c>
+      <c r="D72" s="0" t="n">
+        <v>19177</v>
       </c>
       <c r="E72" s="0" t="n">
+        <v>1393</v>
+      </c>
+      <c r="F72" s="0" t="n">
         <v>33</v>
       </c>
-      <c r="F72" s="0" t="n">
-        <v>38</v>
-      </c>
       <c r="G72" s="0" t="n">
+        <v>38</v>
+      </c>
+      <c r="H72" s="0" t="n">
         <v>3.15</v>
       </c>
-      <c r="H72" s="1" t="s">
-        <v>306</v>
-      </c>
-      <c r="I72" s="0" t="s">
-        <v>313</v>
+      <c r="I72" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="J72" s="0" t="s">
+        <v>256</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="0" t="s">
-        <v>314</v>
+        <v>257</v>
       </c>
       <c r="B73" s="0" t="s">
-        <v>163</v>
-      </c>
-      <c r="D73" s="0" t="s">
-        <v>315</v>
+        <v>133</v>
+      </c>
+      <c r="C73" s="0" t="s">
+        <v>258</v>
+      </c>
+      <c r="D73" s="0" t="n">
+        <v>18784</v>
       </c>
       <c r="E73" s="0" t="n">
+        <v>1759</v>
+      </c>
+      <c r="F73" s="0" t="n">
         <v>35</v>
       </c>
-      <c r="F73" s="0" t="n">
-        <v>38</v>
-      </c>
       <c r="G73" s="0" t="n">
+        <v>38</v>
+      </c>
+      <c r="H73" s="0" t="n">
         <v>3.15</v>
       </c>
-      <c r="H73" s="1" t="s">
-        <v>306</v>
-      </c>
-      <c r="I73" s="0" t="s">
-        <v>316</v>
+      <c r="I73" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="J73" s="0" t="s">
+        <v>259</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="0" t="s">
-        <v>317</v>
+        <v>260</v>
       </c>
       <c r="B74" s="0" t="s">
-        <v>318</v>
+        <v>261</v>
+      </c>
+      <c r="C74" s="0" t="s">
+        <v>262</v>
       </c>
       <c r="D74" s="0" t="s">
-        <v>319</v>
+        <v>38</v>
       </c>
       <c r="E74" s="0" t="n">
+        <v>1829</v>
+      </c>
+      <c r="F74" s="0" t="n">
         <v>35</v>
       </c>
-      <c r="F74" s="0" t="n">
+      <c r="G74" s="0" t="n">
         <v>40</v>
       </c>
-      <c r="G74" s="0" t="n">
+      <c r="H74" s="0" t="n">
         <v>3.15</v>
       </c>
-      <c r="H74" s="1" t="s">
-        <v>306</v>
-      </c>
-      <c r="I74" s="0" t="s">
-        <v>320</v>
+      <c r="I74" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="J74" s="0" t="s">
+        <v>263</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="0" t="s">
-        <v>321</v>
+        <v>264</v>
       </c>
       <c r="B75" s="0" t="s">
-        <v>322</v>
-      </c>
-      <c r="G75" s="0" t="n">
+        <v>265</v>
+      </c>
+      <c r="C75" s="0" t="s">
+        <v>266</v>
+      </c>
+      <c r="D75" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="E75" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="F75" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="G75" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="H75" s="0" t="n">
         <v>3.15</v>
       </c>
-      <c r="H75" s="1" t="s">
-        <v>306</v>
-      </c>
-      <c r="I75" s="0" t="s">
-        <v>323</v>
+      <c r="I75" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="J75" s="0" t="s">
+        <v>267</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="0" t="s">
-        <v>324</v>
+        <v>268</v>
       </c>
       <c r="B76" s="0" t="s">
-        <v>325</v>
-      </c>
-      <c r="G76" s="0" t="n">
+        <v>269</v>
+      </c>
+      <c r="C76" s="0" t="s">
+        <v>270</v>
+      </c>
+      <c r="D76" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="E76" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="F76" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="G76" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="H76" s="0" t="n">
         <v>3.15</v>
       </c>
-      <c r="H76" s="1" t="s">
-        <v>306</v>
-      </c>
-      <c r="I76" s="0" t="s">
-        <v>326</v>
+      <c r="I76" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="J76" s="0" t="s">
+        <v>271</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="0" t="s">
-        <v>327</v>
+        <v>272</v>
       </c>
       <c r="B77" s="0" t="s">
-        <v>101</v>
+        <v>85</v>
+      </c>
+      <c r="C77" s="0" t="s">
+        <v>273</v>
       </c>
       <c r="D77" s="0" t="s">
-        <v>103</v>
+        <v>38</v>
       </c>
       <c r="E77" s="0" t="n">
+        <v>578</v>
+      </c>
+      <c r="F77" s="0" t="n">
         <v>23</v>
       </c>
-      <c r="F77" s="0" t="n">
+      <c r="G77" s="0" t="n">
         <v>25</v>
       </c>
-      <c r="G77" s="0" t="n">
+      <c r="H77" s="0" t="n">
         <v>3.15</v>
       </c>
-      <c r="H77" s="1" t="s">
-        <v>306</v>
-      </c>
-      <c r="I77" s="0" t="s">
-        <v>104</v>
+      <c r="I77" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="J77" s="0" t="s">
+        <v>87</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated 22Q2 EH numbers
</commit_message>
<xml_diff>
--- a/inst/extdata/depmap_datasets_list.xlsx
+++ b/inst/extdata/depmap_datasets_list.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="413" uniqueCount="274">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="448" uniqueCount="294">
   <si>
     <t xml:space="preserve">Dataset</t>
   </si>
@@ -842,6 +842,66 @@
   </si>
   <si>
     <t xml:space="preserve">EH7530</t>
+  </si>
+  <si>
+    <t xml:space="preserve">crispr_22Q2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EH7554</t>
+  </si>
+  <si>
+    <t xml:space="preserve">May 9 2022</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://ndownloader.figshare.com/files/34990036</t>
+  </si>
+  <si>
+    <t xml:space="preserve">copyNumber_22Q2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Inferred log copy number data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EH7555</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://ndownloader.figshare.com/files/34989937</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TPM_22Q2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EH7556</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://ndownloader.figshare.com/files/34989919</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mutationCalls_22Q2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EH7557</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://ndownloader.figshare.com/files/34989940</t>
+  </si>
+  <si>
+    <t xml:space="preserve">metadata_22Q2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EH7558</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://ndownloader.figshare.com/files/35020903</t>
+  </si>
+  <si>
+    <t xml:space="preserve">achilles_22Q2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EH7559</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://ndownloader.figshare.com/files/34989901</t>
   </si>
 </sst>
 </file>
@@ -957,10 +1017,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J77"/>
+  <dimension ref="A1:J83"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A52" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C75" activeCellId="0" sqref="C75"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A63" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B87" activeCellId="0" sqref="B87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3442,6 +3502,198 @@
         <v>87</v>
       </c>
     </row>
+    <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A78" s="0" t="s">
+        <v>274</v>
+      </c>
+      <c r="B78" s="0" t="s">
+        <v>213</v>
+      </c>
+      <c r="C78" s="0" t="s">
+        <v>275</v>
+      </c>
+      <c r="D78" s="0" t="n">
+        <v>17386</v>
+      </c>
+      <c r="E78" s="0" t="n">
+        <v>1086</v>
+      </c>
+      <c r="F78" s="0" t="n">
+        <v>31</v>
+      </c>
+      <c r="G78" s="0" t="n">
+        <v>28</v>
+      </c>
+      <c r="H78" s="0" t="n">
+        <v>3.16</v>
+      </c>
+      <c r="I78" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="J78" s="0" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A79" s="0" t="s">
+        <v>278</v>
+      </c>
+      <c r="B79" s="0" t="s">
+        <v>279</v>
+      </c>
+      <c r="C79" s="0" t="s">
+        <v>280</v>
+      </c>
+      <c r="D79" s="0" t="n">
+        <v>25368</v>
+      </c>
+      <c r="E79" s="0" t="n">
+        <v>1766</v>
+      </c>
+      <c r="F79" s="0" t="n">
+        <v>33</v>
+      </c>
+      <c r="G79" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="H79" s="0" t="n">
+        <v>3.16</v>
+      </c>
+      <c r="I79" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="J79" s="0" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A80" s="0" t="s">
+        <v>282</v>
+      </c>
+      <c r="B80" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="C80" s="0" t="s">
+        <v>283</v>
+      </c>
+      <c r="D80" s="0" t="n">
+        <v>19221</v>
+      </c>
+      <c r="E80" s="0" t="n">
+        <v>1406</v>
+      </c>
+      <c r="F80" s="0" t="n">
+        <v>33</v>
+      </c>
+      <c r="G80" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="H80" s="0" t="n">
+        <v>3.16</v>
+      </c>
+      <c r="I80" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="J80" s="0" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A81" s="0" t="s">
+        <v>285</v>
+      </c>
+      <c r="B81" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="C81" s="0" t="s">
+        <v>286</v>
+      </c>
+      <c r="D81" s="0" t="n">
+        <v>18784</v>
+      </c>
+      <c r="E81" s="0" t="n">
+        <v>1771</v>
+      </c>
+      <c r="F81" s="0" t="n">
+        <v>33</v>
+      </c>
+      <c r="G81" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="H81" s="0" t="n">
+        <v>3.16</v>
+      </c>
+      <c r="I81" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="J81" s="0" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A82" s="0" t="s">
+        <v>288</v>
+      </c>
+      <c r="B82" s="0" t="s">
+        <v>261</v>
+      </c>
+      <c r="C82" s="0" t="s">
+        <v>289</v>
+      </c>
+      <c r="D82" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="E82" s="0" t="n">
+        <v>1840</v>
+      </c>
+      <c r="F82" s="0" t="n">
+        <v>33</v>
+      </c>
+      <c r="G82" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="H82" s="0" t="n">
+        <v>3.16</v>
+      </c>
+      <c r="I82" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="J82" s="0" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A83" s="0" t="s">
+        <v>291</v>
+      </c>
+      <c r="B83" s="0" t="s">
+        <v>265</v>
+      </c>
+      <c r="C83" s="0" t="s">
+        <v>292</v>
+      </c>
+      <c r="D83" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="E83" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="F83" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="G83" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="H83" s="0" t="n">
+        <v>3.16</v>
+      </c>
+      <c r="I83" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="J83" s="0" t="s">
+        <v>293</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>